<commit_message>
Sort Project TC 2
</commit_message>
<xml_diff>
--- a/[1] Build/3조_간트차트_일정관리.xlsx
+++ b/[1] Build/3조_간트차트_일정관리.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5462s\Desktop\Folder\TransCompiler_for_beginner\[1] 구축\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seoil\Desktop\TransCompiler_for_beginner\[1] Build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68797B1C-ADBD-4F35-A550-16453954E822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340456F8-801F-4189-A4B7-8A180544163D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,16 +16,6 @@
     <sheet name="간트 차트 템플릿" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1438,27 +1428,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1466,6 +1466,24 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1476,34 +1494,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1725,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:BQ85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:BP85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1814,44 +1804,44 @@
     </row>
     <row r="2" spans="1:69" ht="41.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="109" t="s">
+      <c r="I2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="110" t="s">
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="108"/>
-      <c r="X2" s="108"/>
-      <c r="Y2" s="108"/>
-      <c r="Z2" s="108"/>
-      <c r="AA2" s="108"/>
-      <c r="AB2" s="108"/>
-      <c r="AC2" s="108"/>
-      <c r="AD2" s="108"/>
-      <c r="AE2" s="108"/>
-      <c r="AF2" s="108"/>
-      <c r="AG2" s="108"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="88"/>
+      <c r="Z2" s="88"/>
+      <c r="AA2" s="88"/>
+      <c r="AB2" s="88"/>
+      <c r="AC2" s="88"/>
+      <c r="AD2" s="88"/>
+      <c r="AE2" s="88"/>
+      <c r="AF2" s="88"/>
+      <c r="AG2" s="88"/>
       <c r="AH2" s="11"/>
       <c r="AI2" s="11"/>
       <c r="AJ2" s="11"/>
@@ -1962,41 +1952,41 @@
     </row>
     <row r="4" spans="1:69" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="111" t="s">
+      <c r="C4" s="92"/>
+      <c r="D4" s="93" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="89" t="s">
+      <c r="I4" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="112" t="s">
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="90"/>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
+      <c r="U4" s="92"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="92"/>
+      <c r="X4" s="92"/>
+      <c r="Y4" s="92"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="92"/>
+      <c r="AB4" s="92"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
@@ -2041,40 +2031,40 @@
     </row>
     <row r="5" spans="1:69" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91" t="s">
+      <c r="C5" s="92"/>
+      <c r="D5" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="89" t="s">
+      <c r="I5" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="92">
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="107">
         <v>44881</v>
       </c>
-      <c r="Q5" s="90"/>
-      <c r="R5" s="90"/>
-      <c r="S5" s="90"/>
-      <c r="T5" s="90"/>
-      <c r="U5" s="90"/>
-      <c r="V5" s="90"/>
-      <c r="W5" s="90"/>
-      <c r="X5" s="90"/>
-      <c r="Y5" s="90"/>
-      <c r="Z5" s="90"/>
-      <c r="AA5" s="90"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="92"/>
+      <c r="S5" s="92"/>
+      <c r="T5" s="92"/>
+      <c r="U5" s="92"/>
+      <c r="V5" s="92"/>
+      <c r="W5" s="92"/>
+      <c r="X5" s="92"/>
+      <c r="Y5" s="92"/>
+      <c r="Z5" s="92"/>
+      <c r="AA5" s="92"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="1"/>
@@ -2337,201 +2327,201 @@
     </row>
     <row r="9" spans="1:69" ht="17.25" customHeight="1">
       <c r="A9" s="25"/>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="93" t="s">
+      <c r="E9" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="93" t="s">
+      <c r="F9" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="93" t="s">
+      <c r="G9" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="93" t="s">
+      <c r="H9" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="106" t="s">
+      <c r="I9" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="94"/>
-      <c r="T9" s="94"/>
-      <c r="U9" s="94"/>
-      <c r="V9" s="94"/>
-      <c r="W9" s="94"/>
-      <c r="X9" s="99" t="s">
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="97"/>
+      <c r="R9" s="97"/>
+      <c r="S9" s="97"/>
+      <c r="T9" s="97"/>
+      <c r="U9" s="97"/>
+      <c r="V9" s="97"/>
+      <c r="W9" s="97"/>
+      <c r="X9" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="Y9" s="94"/>
-      <c r="Z9" s="94"/>
-      <c r="AA9" s="94"/>
-      <c r="AB9" s="94"/>
-      <c r="AC9" s="94"/>
-      <c r="AD9" s="94"/>
-      <c r="AE9" s="94"/>
-      <c r="AF9" s="94"/>
-      <c r="AG9" s="94"/>
-      <c r="AH9" s="94"/>
-      <c r="AI9" s="94"/>
-      <c r="AJ9" s="94"/>
-      <c r="AK9" s="94"/>
-      <c r="AL9" s="94"/>
-      <c r="AM9" s="100" t="s">
+      <c r="Y9" s="97"/>
+      <c r="Z9" s="97"/>
+      <c r="AA9" s="97"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="97"/>
+      <c r="AD9" s="97"/>
+      <c r="AE9" s="97"/>
+      <c r="AF9" s="97"/>
+      <c r="AG9" s="97"/>
+      <c r="AH9" s="97"/>
+      <c r="AI9" s="97"/>
+      <c r="AJ9" s="97"/>
+      <c r="AK9" s="97"/>
+      <c r="AL9" s="97"/>
+      <c r="AM9" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="AN9" s="94"/>
-      <c r="AO9" s="94"/>
-      <c r="AP9" s="94"/>
-      <c r="AQ9" s="94"/>
-      <c r="AR9" s="94"/>
-      <c r="AS9" s="94"/>
-      <c r="AT9" s="94"/>
-      <c r="AU9" s="94"/>
-      <c r="AV9" s="94"/>
-      <c r="AW9" s="94"/>
-      <c r="AX9" s="94"/>
-      <c r="AY9" s="94"/>
-      <c r="AZ9" s="94"/>
-      <c r="BA9" s="94"/>
-      <c r="BB9" s="101" t="s">
+      <c r="AN9" s="97"/>
+      <c r="AO9" s="97"/>
+      <c r="AP9" s="97"/>
+      <c r="AQ9" s="97"/>
+      <c r="AR9" s="97"/>
+      <c r="AS9" s="97"/>
+      <c r="AT9" s="97"/>
+      <c r="AU9" s="97"/>
+      <c r="AV9" s="97"/>
+      <c r="AW9" s="97"/>
+      <c r="AX9" s="97"/>
+      <c r="AY9" s="97"/>
+      <c r="AZ9" s="97"/>
+      <c r="BA9" s="97"/>
+      <c r="BB9" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="BC9" s="94"/>
-      <c r="BD9" s="94"/>
-      <c r="BE9" s="94"/>
-      <c r="BF9" s="94"/>
-      <c r="BG9" s="94"/>
-      <c r="BH9" s="94"/>
-      <c r="BI9" s="94"/>
-      <c r="BJ9" s="94"/>
-      <c r="BK9" s="94"/>
-      <c r="BL9" s="94"/>
-      <c r="BM9" s="94"/>
-      <c r="BN9" s="94"/>
-      <c r="BO9" s="94"/>
-      <c r="BP9" s="102"/>
+      <c r="BC9" s="97"/>
+      <c r="BD9" s="97"/>
+      <c r="BE9" s="97"/>
+      <c r="BF9" s="97"/>
+      <c r="BG9" s="97"/>
+      <c r="BH9" s="97"/>
+      <c r="BI9" s="97"/>
+      <c r="BJ9" s="97"/>
+      <c r="BK9" s="97"/>
+      <c r="BL9" s="97"/>
+      <c r="BM9" s="97"/>
+      <c r="BN9" s="97"/>
+      <c r="BO9" s="97"/>
+      <c r="BP9" s="112"/>
       <c r="BQ9" s="21"/>
     </row>
     <row r="10" spans="1:69" ht="17.25" customHeight="1">
       <c r="A10" s="26"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="95" t="s">
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="97"/>
-      <c r="N10" s="95" t="s">
+      <c r="J10" s="100"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="101"/>
+      <c r="N10" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="96"/>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="97"/>
-      <c r="S10" s="95" t="s">
+      <c r="O10" s="100"/>
+      <c r="P10" s="100"/>
+      <c r="Q10" s="100"/>
+      <c r="R10" s="101"/>
+      <c r="S10" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="T10" s="96"/>
-      <c r="U10" s="96"/>
-      <c r="V10" s="96"/>
-      <c r="W10" s="97"/>
-      <c r="X10" s="98" t="s">
+      <c r="T10" s="100"/>
+      <c r="U10" s="100"/>
+      <c r="V10" s="100"/>
+      <c r="W10" s="101"/>
+      <c r="X10" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="Y10" s="96"/>
-      <c r="Z10" s="96"/>
-      <c r="AA10" s="96"/>
-      <c r="AB10" s="97"/>
-      <c r="AC10" s="98" t="s">
+      <c r="Y10" s="100"/>
+      <c r="Z10" s="100"/>
+      <c r="AA10" s="100"/>
+      <c r="AB10" s="101"/>
+      <c r="AC10" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="AD10" s="96"/>
-      <c r="AE10" s="96"/>
-      <c r="AF10" s="96"/>
-      <c r="AG10" s="97"/>
-      <c r="AH10" s="98" t="s">
+      <c r="AD10" s="100"/>
+      <c r="AE10" s="100"/>
+      <c r="AF10" s="100"/>
+      <c r="AG10" s="101"/>
+      <c r="AH10" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="AI10" s="96"/>
-      <c r="AJ10" s="96"/>
-      <c r="AK10" s="96"/>
-      <c r="AL10" s="97"/>
-      <c r="AM10" s="104" t="s">
+      <c r="AI10" s="100"/>
+      <c r="AJ10" s="100"/>
+      <c r="AK10" s="100"/>
+      <c r="AL10" s="101"/>
+      <c r="AM10" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="AN10" s="96"/>
-      <c r="AO10" s="96"/>
-      <c r="AP10" s="96"/>
-      <c r="AQ10" s="97"/>
-      <c r="AR10" s="104" t="s">
+      <c r="AN10" s="100"/>
+      <c r="AO10" s="100"/>
+      <c r="AP10" s="100"/>
+      <c r="AQ10" s="101"/>
+      <c r="AR10" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="AS10" s="96"/>
-      <c r="AT10" s="96"/>
-      <c r="AU10" s="96"/>
-      <c r="AV10" s="97"/>
-      <c r="AW10" s="104" t="s">
+      <c r="AS10" s="100"/>
+      <c r="AT10" s="100"/>
+      <c r="AU10" s="100"/>
+      <c r="AV10" s="101"/>
+      <c r="AW10" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="AX10" s="96"/>
-      <c r="AY10" s="96"/>
-      <c r="AZ10" s="96"/>
-      <c r="BA10" s="97"/>
-      <c r="BB10" s="103" t="s">
+      <c r="AX10" s="100"/>
+      <c r="AY10" s="100"/>
+      <c r="AZ10" s="100"/>
+      <c r="BA10" s="101"/>
+      <c r="BB10" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="BC10" s="96"/>
-      <c r="BD10" s="96"/>
-      <c r="BE10" s="96"/>
-      <c r="BF10" s="97"/>
-      <c r="BG10" s="103" t="s">
+      <c r="BC10" s="100"/>
+      <c r="BD10" s="100"/>
+      <c r="BE10" s="100"/>
+      <c r="BF10" s="101"/>
+      <c r="BG10" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="BH10" s="96"/>
-      <c r="BI10" s="96"/>
-      <c r="BJ10" s="96"/>
-      <c r="BK10" s="97"/>
-      <c r="BL10" s="103" t="s">
+      <c r="BH10" s="100"/>
+      <c r="BI10" s="100"/>
+      <c r="BJ10" s="100"/>
+      <c r="BK10" s="101"/>
+      <c r="BL10" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="BM10" s="96"/>
-      <c r="BN10" s="96"/>
-      <c r="BO10" s="96"/>
-      <c r="BP10" s="97"/>
+      <c r="BM10" s="100"/>
+      <c r="BN10" s="100"/>
+      <c r="BO10" s="100"/>
+      <c r="BP10" s="101"/>
       <c r="BQ10" s="26"/>
     </row>
     <row r="11" spans="1:69" ht="17.25" customHeight="1">
       <c r="A11" s="27"/>
-      <c r="B11" s="94"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
       <c r="I11" s="28" t="s">
         <v>30</v>
       </c>
@@ -7497,7 +7487,7 @@
         <v>7</v>
       </c>
       <c r="H68" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" s="51"/>
       <c r="J68" s="52"/>
@@ -7583,7 +7573,7 @@
         <v>7</v>
       </c>
       <c r="H69" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69" s="51"/>
       <c r="J69" s="52"/>
@@ -7648,1162 +7638,1143 @@
       <c r="BQ69" s="38"/>
     </row>
     <row r="70" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A70" s="87"/>
-      <c r="B70" s="87"/>
-      <c r="C70" s="87"/>
-      <c r="D70" s="87"/>
-      <c r="E70" s="87"/>
-      <c r="F70" s="87"/>
-      <c r="G70" s="87"/>
-      <c r="H70" s="87"/>
-      <c r="I70" s="87"/>
-      <c r="J70" s="87"/>
-      <c r="K70" s="87"/>
-      <c r="L70" s="87"/>
-      <c r="M70" s="87"/>
-      <c r="N70" s="87"/>
-      <c r="O70" s="87"/>
-      <c r="P70" s="87"/>
-      <c r="Q70" s="87"/>
-      <c r="R70" s="87"/>
-      <c r="S70" s="87"/>
-      <c r="T70" s="87"/>
-      <c r="U70" s="87"/>
-      <c r="V70" s="87"/>
-      <c r="W70" s="87"/>
-      <c r="X70" s="87"/>
-      <c r="Y70" s="87"/>
-      <c r="Z70" s="87"/>
-      <c r="AA70" s="87"/>
-      <c r="AB70" s="87"/>
-      <c r="AC70" s="87"/>
-      <c r="AD70" s="87"/>
-      <c r="AE70" s="87"/>
-      <c r="AF70" s="87"/>
-      <c r="AG70" s="87"/>
-      <c r="AH70" s="87"/>
-      <c r="AI70" s="87"/>
-      <c r="AJ70" s="87"/>
-      <c r="AK70" s="87"/>
-      <c r="AL70" s="87"/>
-      <c r="AM70" s="87"/>
-      <c r="AN70" s="87"/>
-      <c r="AO70" s="87"/>
-      <c r="AP70" s="87"/>
-      <c r="AQ70" s="87"/>
-      <c r="AR70" s="87"/>
-      <c r="AS70" s="87"/>
-      <c r="AT70" s="87"/>
-      <c r="AU70" s="87"/>
-      <c r="AV70" s="87"/>
-      <c r="AW70" s="87"/>
-      <c r="AX70" s="87"/>
-      <c r="AY70" s="87"/>
-      <c r="AZ70" s="87"/>
-      <c r="BA70" s="87"/>
-      <c r="BB70" s="87"/>
-      <c r="BC70" s="87"/>
-      <c r="BD70" s="87"/>
-      <c r="BE70" s="87"/>
-      <c r="BF70" s="87"/>
-      <c r="BG70" s="87"/>
-      <c r="BH70" s="87"/>
-      <c r="BI70" s="87"/>
-      <c r="BJ70" s="87"/>
-      <c r="BK70" s="87"/>
-      <c r="BL70" s="87"/>
-      <c r="BM70" s="87"/>
-      <c r="BN70" s="87"/>
-      <c r="BO70" s="87"/>
-      <c r="BP70" s="88"/>
+      <c r="A70" s="104"/>
+      <c r="B70" s="104"/>
+      <c r="C70" s="104"/>
+      <c r="D70" s="104"/>
+      <c r="E70" s="104"/>
+      <c r="F70" s="104"/>
+      <c r="G70" s="104"/>
+      <c r="H70" s="104"/>
+      <c r="I70" s="104"/>
+      <c r="J70" s="104"/>
+      <c r="K70" s="104"/>
+      <c r="L70" s="104"/>
+      <c r="M70" s="104"/>
+      <c r="N70" s="104"/>
+      <c r="O70" s="104"/>
+      <c r="P70" s="104"/>
+      <c r="Q70" s="104"/>
+      <c r="R70" s="104"/>
+      <c r="S70" s="104"/>
+      <c r="T70" s="104"/>
+      <c r="U70" s="104"/>
+      <c r="V70" s="104"/>
+      <c r="W70" s="104"/>
+      <c r="X70" s="104"/>
+      <c r="Y70" s="104"/>
+      <c r="Z70" s="104"/>
+      <c r="AA70" s="104"/>
+      <c r="AB70" s="104"/>
+      <c r="AC70" s="104"/>
+      <c r="AD70" s="104"/>
+      <c r="AE70" s="104"/>
+      <c r="AF70" s="104"/>
+      <c r="AG70" s="104"/>
+      <c r="AH70" s="104"/>
+      <c r="AI70" s="104"/>
+      <c r="AJ70" s="104"/>
+      <c r="AK70" s="104"/>
+      <c r="AL70" s="104"/>
+      <c r="AM70" s="104"/>
+      <c r="AN70" s="104"/>
+      <c r="AO70" s="104"/>
+      <c r="AP70" s="104"/>
+      <c r="AQ70" s="104"/>
+      <c r="AR70" s="104"/>
+      <c r="AS70" s="104"/>
+      <c r="AT70" s="104"/>
+      <c r="AU70" s="104"/>
+      <c r="AV70" s="104"/>
+      <c r="AW70" s="104"/>
+      <c r="AX70" s="104"/>
+      <c r="AY70" s="104"/>
+      <c r="AZ70" s="104"/>
+      <c r="BA70" s="104"/>
+      <c r="BB70" s="104"/>
+      <c r="BC70" s="104"/>
+      <c r="BD70" s="104"/>
+      <c r="BE70" s="104"/>
+      <c r="BF70" s="104"/>
+      <c r="BG70" s="104"/>
+      <c r="BH70" s="104"/>
+      <c r="BI70" s="104"/>
+      <c r="BJ70" s="104"/>
+      <c r="BK70" s="104"/>
+      <c r="BL70" s="104"/>
+      <c r="BM70" s="104"/>
+      <c r="BN70" s="104"/>
+      <c r="BO70" s="104"/>
+      <c r="BP70" s="105"/>
       <c r="BQ70" s="38"/>
     </row>
     <row r="71" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A71" s="87"/>
-      <c r="B71" s="87"/>
-      <c r="C71" s="87"/>
-      <c r="D71" s="87"/>
-      <c r="E71" s="87"/>
-      <c r="F71" s="87"/>
-      <c r="G71" s="87"/>
-      <c r="H71" s="87"/>
-      <c r="I71" s="87"/>
-      <c r="J71" s="87"/>
-      <c r="K71" s="87"/>
-      <c r="L71" s="87"/>
-      <c r="M71" s="87"/>
-      <c r="N71" s="87"/>
-      <c r="O71" s="87"/>
-      <c r="P71" s="87"/>
-      <c r="Q71" s="87"/>
-      <c r="R71" s="87"/>
-      <c r="S71" s="87"/>
-      <c r="T71" s="87"/>
-      <c r="U71" s="87"/>
-      <c r="V71" s="87"/>
-      <c r="W71" s="87"/>
-      <c r="X71" s="87"/>
-      <c r="Y71" s="87"/>
-      <c r="Z71" s="87"/>
-      <c r="AA71" s="87"/>
-      <c r="AB71" s="87"/>
-      <c r="AC71" s="87"/>
-      <c r="AD71" s="87"/>
-      <c r="AE71" s="87"/>
-      <c r="AF71" s="87"/>
-      <c r="AG71" s="87"/>
-      <c r="AH71" s="87"/>
-      <c r="AI71" s="87"/>
-      <c r="AJ71" s="87"/>
-      <c r="AK71" s="87"/>
-      <c r="AL71" s="87"/>
-      <c r="AM71" s="87"/>
-      <c r="AN71" s="87"/>
-      <c r="AO71" s="87"/>
-      <c r="AP71" s="87"/>
-      <c r="AQ71" s="87"/>
-      <c r="AR71" s="87"/>
-      <c r="AS71" s="87"/>
-      <c r="AT71" s="87"/>
-      <c r="AU71" s="87"/>
-      <c r="AV71" s="87"/>
-      <c r="AW71" s="87"/>
-      <c r="AX71" s="87"/>
-      <c r="AY71" s="87"/>
-      <c r="AZ71" s="87"/>
-      <c r="BA71" s="87"/>
-      <c r="BB71" s="87"/>
-      <c r="BC71" s="87"/>
-      <c r="BD71" s="87"/>
-      <c r="BE71" s="87"/>
-      <c r="BF71" s="87"/>
-      <c r="BG71" s="87"/>
-      <c r="BH71" s="87"/>
-      <c r="BI71" s="87"/>
-      <c r="BJ71" s="87"/>
-      <c r="BK71" s="87"/>
-      <c r="BL71" s="87"/>
-      <c r="BM71" s="87"/>
-      <c r="BN71" s="87"/>
-      <c r="BO71" s="87"/>
-      <c r="BP71" s="88"/>
+      <c r="A71" s="104"/>
+      <c r="B71" s="104"/>
+      <c r="C71" s="104"/>
+      <c r="D71" s="104"/>
+      <c r="E71" s="104"/>
+      <c r="F71" s="104"/>
+      <c r="G71" s="104"/>
+      <c r="H71" s="104"/>
+      <c r="I71" s="104"/>
+      <c r="J71" s="104"/>
+      <c r="K71" s="104"/>
+      <c r="L71" s="104"/>
+      <c r="M71" s="104"/>
+      <c r="N71" s="104"/>
+      <c r="O71" s="104"/>
+      <c r="P71" s="104"/>
+      <c r="Q71" s="104"/>
+      <c r="R71" s="104"/>
+      <c r="S71" s="104"/>
+      <c r="T71" s="104"/>
+      <c r="U71" s="104"/>
+      <c r="V71" s="104"/>
+      <c r="W71" s="104"/>
+      <c r="X71" s="104"/>
+      <c r="Y71" s="104"/>
+      <c r="Z71" s="104"/>
+      <c r="AA71" s="104"/>
+      <c r="AB71" s="104"/>
+      <c r="AC71" s="104"/>
+      <c r="AD71" s="104"/>
+      <c r="AE71" s="104"/>
+      <c r="AF71" s="104"/>
+      <c r="AG71" s="104"/>
+      <c r="AH71" s="104"/>
+      <c r="AI71" s="104"/>
+      <c r="AJ71" s="104"/>
+      <c r="AK71" s="104"/>
+      <c r="AL71" s="104"/>
+      <c r="AM71" s="104"/>
+      <c r="AN71" s="104"/>
+      <c r="AO71" s="104"/>
+      <c r="AP71" s="104"/>
+      <c r="AQ71" s="104"/>
+      <c r="AR71" s="104"/>
+      <c r="AS71" s="104"/>
+      <c r="AT71" s="104"/>
+      <c r="AU71" s="104"/>
+      <c r="AV71" s="104"/>
+      <c r="AW71" s="104"/>
+      <c r="AX71" s="104"/>
+      <c r="AY71" s="104"/>
+      <c r="AZ71" s="104"/>
+      <c r="BA71" s="104"/>
+      <c r="BB71" s="104"/>
+      <c r="BC71" s="104"/>
+      <c r="BD71" s="104"/>
+      <c r="BE71" s="104"/>
+      <c r="BF71" s="104"/>
+      <c r="BG71" s="104"/>
+      <c r="BH71" s="104"/>
+      <c r="BI71" s="104"/>
+      <c r="BJ71" s="104"/>
+      <c r="BK71" s="104"/>
+      <c r="BL71" s="104"/>
+      <c r="BM71" s="104"/>
+      <c r="BN71" s="104"/>
+      <c r="BO71" s="104"/>
+      <c r="BP71" s="105"/>
       <c r="BQ71" s="38"/>
     </row>
     <row r="72" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A72" s="87"/>
-      <c r="B72" s="87"/>
-      <c r="C72" s="87"/>
-      <c r="D72" s="87"/>
-      <c r="E72" s="87"/>
-      <c r="F72" s="87"/>
-      <c r="G72" s="87"/>
-      <c r="H72" s="87"/>
-      <c r="I72" s="87"/>
-      <c r="J72" s="87"/>
-      <c r="K72" s="87"/>
-      <c r="L72" s="87"/>
-      <c r="M72" s="87"/>
-      <c r="N72" s="87"/>
-      <c r="O72" s="87"/>
-      <c r="P72" s="87"/>
-      <c r="Q72" s="87"/>
-      <c r="R72" s="87"/>
-      <c r="S72" s="87"/>
-      <c r="T72" s="87"/>
-      <c r="U72" s="87"/>
-      <c r="V72" s="87"/>
-      <c r="W72" s="87"/>
-      <c r="X72" s="87"/>
-      <c r="Y72" s="87"/>
-      <c r="Z72" s="87"/>
-      <c r="AA72" s="87"/>
-      <c r="AB72" s="87"/>
-      <c r="AC72" s="87"/>
-      <c r="AD72" s="87"/>
-      <c r="AE72" s="87"/>
-      <c r="AF72" s="87"/>
-      <c r="AG72" s="87"/>
-      <c r="AH72" s="87"/>
-      <c r="AI72" s="87"/>
-      <c r="AJ72" s="87"/>
-      <c r="AK72" s="87"/>
-      <c r="AL72" s="87"/>
-      <c r="AM72" s="87"/>
-      <c r="AN72" s="87"/>
-      <c r="AO72" s="87"/>
-      <c r="AP72" s="87"/>
-      <c r="AQ72" s="87"/>
-      <c r="AR72" s="87"/>
-      <c r="AS72" s="87"/>
-      <c r="AT72" s="87"/>
-      <c r="AU72" s="87"/>
-      <c r="AV72" s="87"/>
-      <c r="AW72" s="87"/>
-      <c r="AX72" s="87"/>
-      <c r="AY72" s="87"/>
-      <c r="AZ72" s="87"/>
-      <c r="BA72" s="87"/>
-      <c r="BB72" s="87"/>
-      <c r="BC72" s="87"/>
-      <c r="BD72" s="87"/>
-      <c r="BE72" s="87"/>
-      <c r="BF72" s="87"/>
-      <c r="BG72" s="87"/>
-      <c r="BH72" s="87"/>
-      <c r="BI72" s="87"/>
-      <c r="BJ72" s="87"/>
-      <c r="BK72" s="87"/>
-      <c r="BL72" s="87"/>
-      <c r="BM72" s="87"/>
-      <c r="BN72" s="87"/>
-      <c r="BO72" s="87"/>
-      <c r="BP72" s="88"/>
+      <c r="A72" s="104"/>
+      <c r="B72" s="104"/>
+      <c r="C72" s="104"/>
+      <c r="D72" s="104"/>
+      <c r="E72" s="104"/>
+      <c r="F72" s="104"/>
+      <c r="G72" s="104"/>
+      <c r="H72" s="104"/>
+      <c r="I72" s="104"/>
+      <c r="J72" s="104"/>
+      <c r="K72" s="104"/>
+      <c r="L72" s="104"/>
+      <c r="M72" s="104"/>
+      <c r="N72" s="104"/>
+      <c r="O72" s="104"/>
+      <c r="P72" s="104"/>
+      <c r="Q72" s="104"/>
+      <c r="R72" s="104"/>
+      <c r="S72" s="104"/>
+      <c r="T72" s="104"/>
+      <c r="U72" s="104"/>
+      <c r="V72" s="104"/>
+      <c r="W72" s="104"/>
+      <c r="X72" s="104"/>
+      <c r="Y72" s="104"/>
+      <c r="Z72" s="104"/>
+      <c r="AA72" s="104"/>
+      <c r="AB72" s="104"/>
+      <c r="AC72" s="104"/>
+      <c r="AD72" s="104"/>
+      <c r="AE72" s="104"/>
+      <c r="AF72" s="104"/>
+      <c r="AG72" s="104"/>
+      <c r="AH72" s="104"/>
+      <c r="AI72" s="104"/>
+      <c r="AJ72" s="104"/>
+      <c r="AK72" s="104"/>
+      <c r="AL72" s="104"/>
+      <c r="AM72" s="104"/>
+      <c r="AN72" s="104"/>
+      <c r="AO72" s="104"/>
+      <c r="AP72" s="104"/>
+      <c r="AQ72" s="104"/>
+      <c r="AR72" s="104"/>
+      <c r="AS72" s="104"/>
+      <c r="AT72" s="104"/>
+      <c r="AU72" s="104"/>
+      <c r="AV72" s="104"/>
+      <c r="AW72" s="104"/>
+      <c r="AX72" s="104"/>
+      <c r="AY72" s="104"/>
+      <c r="AZ72" s="104"/>
+      <c r="BA72" s="104"/>
+      <c r="BB72" s="104"/>
+      <c r="BC72" s="104"/>
+      <c r="BD72" s="104"/>
+      <c r="BE72" s="104"/>
+      <c r="BF72" s="104"/>
+      <c r="BG72" s="104"/>
+      <c r="BH72" s="104"/>
+      <c r="BI72" s="104"/>
+      <c r="BJ72" s="104"/>
+      <c r="BK72" s="104"/>
+      <c r="BL72" s="104"/>
+      <c r="BM72" s="104"/>
+      <c r="BN72" s="104"/>
+      <c r="BO72" s="104"/>
+      <c r="BP72" s="105"/>
       <c r="BQ72" s="38"/>
     </row>
     <row r="73" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A73" s="87"/>
-      <c r="B73" s="87"/>
-      <c r="C73" s="87"/>
-      <c r="D73" s="87"/>
-      <c r="E73" s="87"/>
-      <c r="F73" s="87"/>
-      <c r="G73" s="87"/>
-      <c r="H73" s="87"/>
-      <c r="I73" s="87"/>
-      <c r="J73" s="87"/>
-      <c r="K73" s="87"/>
-      <c r="L73" s="87"/>
-      <c r="M73" s="87"/>
-      <c r="N73" s="87"/>
-      <c r="O73" s="87"/>
-      <c r="P73" s="87"/>
-      <c r="Q73" s="87"/>
-      <c r="R73" s="87"/>
-      <c r="S73" s="87"/>
-      <c r="T73" s="87"/>
-      <c r="U73" s="87"/>
-      <c r="V73" s="87"/>
-      <c r="W73" s="87"/>
-      <c r="X73" s="87"/>
-      <c r="Y73" s="87"/>
-      <c r="Z73" s="87"/>
-      <c r="AA73" s="87"/>
-      <c r="AB73" s="87"/>
-      <c r="AC73" s="87"/>
-      <c r="AD73" s="87"/>
-      <c r="AE73" s="87"/>
-      <c r="AF73" s="87"/>
-      <c r="AG73" s="87"/>
-      <c r="AH73" s="87"/>
-      <c r="AI73" s="87"/>
-      <c r="AJ73" s="87"/>
-      <c r="AK73" s="87"/>
-      <c r="AL73" s="87"/>
-      <c r="AM73" s="87"/>
-      <c r="AN73" s="87"/>
-      <c r="AO73" s="87"/>
-      <c r="AP73" s="87"/>
-      <c r="AQ73" s="87"/>
-      <c r="AR73" s="87"/>
-      <c r="AS73" s="87"/>
-      <c r="AT73" s="87"/>
-      <c r="AU73" s="87"/>
-      <c r="AV73" s="87"/>
-      <c r="AW73" s="87"/>
-      <c r="AX73" s="87"/>
-      <c r="AY73" s="87"/>
-      <c r="AZ73" s="87"/>
-      <c r="BA73" s="87"/>
-      <c r="BB73" s="87"/>
-      <c r="BC73" s="87"/>
-      <c r="BD73" s="87"/>
-      <c r="BE73" s="87"/>
-      <c r="BF73" s="87"/>
-      <c r="BG73" s="87"/>
-      <c r="BH73" s="87"/>
-      <c r="BI73" s="87"/>
-      <c r="BJ73" s="87"/>
-      <c r="BK73" s="87"/>
-      <c r="BL73" s="87"/>
-      <c r="BM73" s="87"/>
-      <c r="BN73" s="87"/>
-      <c r="BO73" s="87"/>
-      <c r="BP73" s="88"/>
+      <c r="A73" s="104"/>
+      <c r="B73" s="104"/>
+      <c r="C73" s="104"/>
+      <c r="D73" s="104"/>
+      <c r="E73" s="104"/>
+      <c r="F73" s="104"/>
+      <c r="G73" s="104"/>
+      <c r="H73" s="104"/>
+      <c r="I73" s="104"/>
+      <c r="J73" s="104"/>
+      <c r="K73" s="104"/>
+      <c r="L73" s="104"/>
+      <c r="M73" s="104"/>
+      <c r="N73" s="104"/>
+      <c r="O73" s="104"/>
+      <c r="P73" s="104"/>
+      <c r="Q73" s="104"/>
+      <c r="R73" s="104"/>
+      <c r="S73" s="104"/>
+      <c r="T73" s="104"/>
+      <c r="U73" s="104"/>
+      <c r="V73" s="104"/>
+      <c r="W73" s="104"/>
+      <c r="X73" s="104"/>
+      <c r="Y73" s="104"/>
+      <c r="Z73" s="104"/>
+      <c r="AA73" s="104"/>
+      <c r="AB73" s="104"/>
+      <c r="AC73" s="104"/>
+      <c r="AD73" s="104"/>
+      <c r="AE73" s="104"/>
+      <c r="AF73" s="104"/>
+      <c r="AG73" s="104"/>
+      <c r="AH73" s="104"/>
+      <c r="AI73" s="104"/>
+      <c r="AJ73" s="104"/>
+      <c r="AK73" s="104"/>
+      <c r="AL73" s="104"/>
+      <c r="AM73" s="104"/>
+      <c r="AN73" s="104"/>
+      <c r="AO73" s="104"/>
+      <c r="AP73" s="104"/>
+      <c r="AQ73" s="104"/>
+      <c r="AR73" s="104"/>
+      <c r="AS73" s="104"/>
+      <c r="AT73" s="104"/>
+      <c r="AU73" s="104"/>
+      <c r="AV73" s="104"/>
+      <c r="AW73" s="104"/>
+      <c r="AX73" s="104"/>
+      <c r="AY73" s="104"/>
+      <c r="AZ73" s="104"/>
+      <c r="BA73" s="104"/>
+      <c r="BB73" s="104"/>
+      <c r="BC73" s="104"/>
+      <c r="BD73" s="104"/>
+      <c r="BE73" s="104"/>
+      <c r="BF73" s="104"/>
+      <c r="BG73" s="104"/>
+      <c r="BH73" s="104"/>
+      <c r="BI73" s="104"/>
+      <c r="BJ73" s="104"/>
+      <c r="BK73" s="104"/>
+      <c r="BL73" s="104"/>
+      <c r="BM73" s="104"/>
+      <c r="BN73" s="104"/>
+      <c r="BO73" s="104"/>
+      <c r="BP73" s="105"/>
       <c r="BQ73" s="38"/>
     </row>
     <row r="74" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A74" s="87"/>
-      <c r="B74" s="87"/>
-      <c r="C74" s="87"/>
-      <c r="D74" s="87"/>
-      <c r="E74" s="87"/>
-      <c r="F74" s="87"/>
-      <c r="G74" s="87"/>
-      <c r="H74" s="87"/>
-      <c r="I74" s="87"/>
-      <c r="J74" s="87"/>
-      <c r="K74" s="87"/>
-      <c r="L74" s="87"/>
-      <c r="M74" s="87"/>
-      <c r="N74" s="87"/>
-      <c r="O74" s="87"/>
-      <c r="P74" s="87"/>
-      <c r="Q74" s="87"/>
-      <c r="R74" s="87"/>
-      <c r="S74" s="87"/>
-      <c r="T74" s="87"/>
-      <c r="U74" s="87"/>
-      <c r="V74" s="87"/>
-      <c r="W74" s="87"/>
-      <c r="X74" s="87"/>
-      <c r="Y74" s="87"/>
-      <c r="Z74" s="87"/>
-      <c r="AA74" s="87"/>
-      <c r="AB74" s="87"/>
-      <c r="AC74" s="87"/>
-      <c r="AD74" s="87"/>
-      <c r="AE74" s="87"/>
-      <c r="AF74" s="87"/>
-      <c r="AG74" s="87"/>
-      <c r="AH74" s="87"/>
-      <c r="AI74" s="87"/>
-      <c r="AJ74" s="87"/>
-      <c r="AK74" s="87"/>
-      <c r="AL74" s="87"/>
-      <c r="AM74" s="87"/>
-      <c r="AN74" s="87"/>
-      <c r="AO74" s="87"/>
-      <c r="AP74" s="87"/>
-      <c r="AQ74" s="87"/>
-      <c r="AR74" s="87"/>
-      <c r="AS74" s="87"/>
-      <c r="AT74" s="87"/>
-      <c r="AU74" s="87"/>
-      <c r="AV74" s="87"/>
-      <c r="AW74" s="87"/>
-      <c r="AX74" s="87"/>
-      <c r="AY74" s="87"/>
-      <c r="AZ74" s="87"/>
-      <c r="BA74" s="87"/>
-      <c r="BB74" s="87"/>
-      <c r="BC74" s="87"/>
-      <c r="BD74" s="87"/>
-      <c r="BE74" s="87"/>
-      <c r="BF74" s="87"/>
-      <c r="BG74" s="87"/>
-      <c r="BH74" s="87"/>
-      <c r="BI74" s="87"/>
-      <c r="BJ74" s="87"/>
-      <c r="BK74" s="87"/>
-      <c r="BL74" s="87"/>
-      <c r="BM74" s="87"/>
-      <c r="BN74" s="87"/>
-      <c r="BO74" s="87"/>
-      <c r="BP74" s="88"/>
+      <c r="A74" s="104"/>
+      <c r="B74" s="104"/>
+      <c r="C74" s="104"/>
+      <c r="D74" s="104"/>
+      <c r="E74" s="104"/>
+      <c r="F74" s="104"/>
+      <c r="G74" s="104"/>
+      <c r="H74" s="104"/>
+      <c r="I74" s="104"/>
+      <c r="J74" s="104"/>
+      <c r="K74" s="104"/>
+      <c r="L74" s="104"/>
+      <c r="M74" s="104"/>
+      <c r="N74" s="104"/>
+      <c r="O74" s="104"/>
+      <c r="P74" s="104"/>
+      <c r="Q74" s="104"/>
+      <c r="R74" s="104"/>
+      <c r="S74" s="104"/>
+      <c r="T74" s="104"/>
+      <c r="U74" s="104"/>
+      <c r="V74" s="104"/>
+      <c r="W74" s="104"/>
+      <c r="X74" s="104"/>
+      <c r="Y74" s="104"/>
+      <c r="Z74" s="104"/>
+      <c r="AA74" s="104"/>
+      <c r="AB74" s="104"/>
+      <c r="AC74" s="104"/>
+      <c r="AD74" s="104"/>
+      <c r="AE74" s="104"/>
+      <c r="AF74" s="104"/>
+      <c r="AG74" s="104"/>
+      <c r="AH74" s="104"/>
+      <c r="AI74" s="104"/>
+      <c r="AJ74" s="104"/>
+      <c r="AK74" s="104"/>
+      <c r="AL74" s="104"/>
+      <c r="AM74" s="104"/>
+      <c r="AN74" s="104"/>
+      <c r="AO74" s="104"/>
+      <c r="AP74" s="104"/>
+      <c r="AQ74" s="104"/>
+      <c r="AR74" s="104"/>
+      <c r="AS74" s="104"/>
+      <c r="AT74" s="104"/>
+      <c r="AU74" s="104"/>
+      <c r="AV74" s="104"/>
+      <c r="AW74" s="104"/>
+      <c r="AX74" s="104"/>
+      <c r="AY74" s="104"/>
+      <c r="AZ74" s="104"/>
+      <c r="BA74" s="104"/>
+      <c r="BB74" s="104"/>
+      <c r="BC74" s="104"/>
+      <c r="BD74" s="104"/>
+      <c r="BE74" s="104"/>
+      <c r="BF74" s="104"/>
+      <c r="BG74" s="104"/>
+      <c r="BH74" s="104"/>
+      <c r="BI74" s="104"/>
+      <c r="BJ74" s="104"/>
+      <c r="BK74" s="104"/>
+      <c r="BL74" s="104"/>
+      <c r="BM74" s="104"/>
+      <c r="BN74" s="104"/>
+      <c r="BO74" s="104"/>
+      <c r="BP74" s="105"/>
       <c r="BQ74" s="38"/>
     </row>
     <row r="75" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A75" s="87"/>
-      <c r="B75" s="87"/>
-      <c r="C75" s="87"/>
-      <c r="D75" s="87"/>
-      <c r="E75" s="87"/>
-      <c r="F75" s="87"/>
-      <c r="G75" s="87"/>
-      <c r="H75" s="87"/>
-      <c r="I75" s="87"/>
-      <c r="J75" s="87"/>
-      <c r="K75" s="87"/>
-      <c r="L75" s="87"/>
-      <c r="M75" s="87"/>
-      <c r="N75" s="87"/>
-      <c r="O75" s="87"/>
-      <c r="P75" s="87"/>
-      <c r="Q75" s="87"/>
-      <c r="R75" s="87"/>
-      <c r="S75" s="87"/>
-      <c r="T75" s="87"/>
-      <c r="U75" s="87"/>
-      <c r="V75" s="87"/>
-      <c r="W75" s="87"/>
-      <c r="X75" s="87"/>
-      <c r="Y75" s="87"/>
-      <c r="Z75" s="87"/>
-      <c r="AA75" s="87"/>
-      <c r="AB75" s="87"/>
-      <c r="AC75" s="87"/>
-      <c r="AD75" s="87"/>
-      <c r="AE75" s="87"/>
-      <c r="AF75" s="87"/>
-      <c r="AG75" s="87"/>
-      <c r="AH75" s="87"/>
-      <c r="AI75" s="87"/>
-      <c r="AJ75" s="87"/>
-      <c r="AK75" s="87"/>
-      <c r="AL75" s="87"/>
-      <c r="AM75" s="87"/>
-      <c r="AN75" s="87"/>
-      <c r="AO75" s="87"/>
-      <c r="AP75" s="87"/>
-      <c r="AQ75" s="87"/>
-      <c r="AR75" s="87"/>
-      <c r="AS75" s="87"/>
-      <c r="AT75" s="87"/>
-      <c r="AU75" s="87"/>
-      <c r="AV75" s="87"/>
-      <c r="AW75" s="87"/>
-      <c r="AX75" s="87"/>
-      <c r="AY75" s="87"/>
-      <c r="AZ75" s="87"/>
-      <c r="BA75" s="87"/>
-      <c r="BB75" s="87"/>
-      <c r="BC75" s="87"/>
-      <c r="BD75" s="87"/>
-      <c r="BE75" s="87"/>
-      <c r="BF75" s="87"/>
-      <c r="BG75" s="87"/>
-      <c r="BH75" s="87"/>
-      <c r="BI75" s="87"/>
-      <c r="BJ75" s="87"/>
-      <c r="BK75" s="87"/>
-      <c r="BL75" s="87"/>
-      <c r="BM75" s="87"/>
-      <c r="BN75" s="87"/>
-      <c r="BO75" s="87"/>
-      <c r="BP75" s="88"/>
+      <c r="A75" s="104"/>
+      <c r="B75" s="104"/>
+      <c r="C75" s="104"/>
+      <c r="D75" s="104"/>
+      <c r="E75" s="104"/>
+      <c r="F75" s="104"/>
+      <c r="G75" s="104"/>
+      <c r="H75" s="104"/>
+      <c r="I75" s="104"/>
+      <c r="J75" s="104"/>
+      <c r="K75" s="104"/>
+      <c r="L75" s="104"/>
+      <c r="M75" s="104"/>
+      <c r="N75" s="104"/>
+      <c r="O75" s="104"/>
+      <c r="P75" s="104"/>
+      <c r="Q75" s="104"/>
+      <c r="R75" s="104"/>
+      <c r="S75" s="104"/>
+      <c r="T75" s="104"/>
+      <c r="U75" s="104"/>
+      <c r="V75" s="104"/>
+      <c r="W75" s="104"/>
+      <c r="X75" s="104"/>
+      <c r="Y75" s="104"/>
+      <c r="Z75" s="104"/>
+      <c r="AA75" s="104"/>
+      <c r="AB75" s="104"/>
+      <c r="AC75" s="104"/>
+      <c r="AD75" s="104"/>
+      <c r="AE75" s="104"/>
+      <c r="AF75" s="104"/>
+      <c r="AG75" s="104"/>
+      <c r="AH75" s="104"/>
+      <c r="AI75" s="104"/>
+      <c r="AJ75" s="104"/>
+      <c r="AK75" s="104"/>
+      <c r="AL75" s="104"/>
+      <c r="AM75" s="104"/>
+      <c r="AN75" s="104"/>
+      <c r="AO75" s="104"/>
+      <c r="AP75" s="104"/>
+      <c r="AQ75" s="104"/>
+      <c r="AR75" s="104"/>
+      <c r="AS75" s="104"/>
+      <c r="AT75" s="104"/>
+      <c r="AU75" s="104"/>
+      <c r="AV75" s="104"/>
+      <c r="AW75" s="104"/>
+      <c r="AX75" s="104"/>
+      <c r="AY75" s="104"/>
+      <c r="AZ75" s="104"/>
+      <c r="BA75" s="104"/>
+      <c r="BB75" s="104"/>
+      <c r="BC75" s="104"/>
+      <c r="BD75" s="104"/>
+      <c r="BE75" s="104"/>
+      <c r="BF75" s="104"/>
+      <c r="BG75" s="104"/>
+      <c r="BH75" s="104"/>
+      <c r="BI75" s="104"/>
+      <c r="BJ75" s="104"/>
+      <c r="BK75" s="104"/>
+      <c r="BL75" s="104"/>
+      <c r="BM75" s="104"/>
+      <c r="BN75" s="104"/>
+      <c r="BO75" s="104"/>
+      <c r="BP75" s="105"/>
       <c r="BQ75" s="38"/>
     </row>
     <row r="76" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A76" s="87"/>
-      <c r="B76" s="87"/>
-      <c r="C76" s="87"/>
-      <c r="D76" s="87"/>
-      <c r="E76" s="87"/>
-      <c r="F76" s="87"/>
-      <c r="G76" s="87"/>
-      <c r="H76" s="87"/>
-      <c r="I76" s="87"/>
-      <c r="J76" s="87"/>
-      <c r="K76" s="87"/>
-      <c r="L76" s="87"/>
-      <c r="M76" s="87"/>
-      <c r="N76" s="87"/>
-      <c r="O76" s="87"/>
-      <c r="P76" s="87"/>
-      <c r="Q76" s="87"/>
-      <c r="R76" s="87"/>
-      <c r="S76" s="87"/>
-      <c r="T76" s="87"/>
-      <c r="U76" s="87"/>
-      <c r="V76" s="87"/>
-      <c r="W76" s="87"/>
-      <c r="X76" s="87"/>
-      <c r="Y76" s="87"/>
-      <c r="Z76" s="87"/>
-      <c r="AA76" s="87"/>
-      <c r="AB76" s="87"/>
-      <c r="AC76" s="87"/>
-      <c r="AD76" s="87"/>
-      <c r="AE76" s="87"/>
-      <c r="AF76" s="87"/>
-      <c r="AG76" s="87"/>
-      <c r="AH76" s="87"/>
-      <c r="AI76" s="87"/>
-      <c r="AJ76" s="87"/>
-      <c r="AK76" s="87"/>
-      <c r="AL76" s="87"/>
-      <c r="AM76" s="87"/>
-      <c r="AN76" s="87"/>
-      <c r="AO76" s="87"/>
-      <c r="AP76" s="87"/>
-      <c r="AQ76" s="87"/>
-      <c r="AR76" s="87"/>
-      <c r="AS76" s="87"/>
-      <c r="AT76" s="87"/>
-      <c r="AU76" s="87"/>
-      <c r="AV76" s="87"/>
-      <c r="AW76" s="87"/>
-      <c r="AX76" s="87"/>
-      <c r="AY76" s="87"/>
-      <c r="AZ76" s="87"/>
-      <c r="BA76" s="87"/>
-      <c r="BB76" s="87"/>
-      <c r="BC76" s="87"/>
-      <c r="BD76" s="87"/>
-      <c r="BE76" s="87"/>
-      <c r="BF76" s="87"/>
-      <c r="BG76" s="87"/>
-      <c r="BH76" s="87"/>
-      <c r="BI76" s="87"/>
-      <c r="BJ76" s="87"/>
-      <c r="BK76" s="87"/>
-      <c r="BL76" s="87"/>
-      <c r="BM76" s="87"/>
-      <c r="BN76" s="87"/>
-      <c r="BO76" s="87"/>
-      <c r="BP76" s="88"/>
+      <c r="A76" s="104"/>
+      <c r="B76" s="104"/>
+      <c r="C76" s="104"/>
+      <c r="D76" s="104"/>
+      <c r="E76" s="104"/>
+      <c r="F76" s="104"/>
+      <c r="G76" s="104"/>
+      <c r="H76" s="104"/>
+      <c r="I76" s="104"/>
+      <c r="J76" s="104"/>
+      <c r="K76" s="104"/>
+      <c r="L76" s="104"/>
+      <c r="M76" s="104"/>
+      <c r="N76" s="104"/>
+      <c r="O76" s="104"/>
+      <c r="P76" s="104"/>
+      <c r="Q76" s="104"/>
+      <c r="R76" s="104"/>
+      <c r="S76" s="104"/>
+      <c r="T76" s="104"/>
+      <c r="U76" s="104"/>
+      <c r="V76" s="104"/>
+      <c r="W76" s="104"/>
+      <c r="X76" s="104"/>
+      <c r="Y76" s="104"/>
+      <c r="Z76" s="104"/>
+      <c r="AA76" s="104"/>
+      <c r="AB76" s="104"/>
+      <c r="AC76" s="104"/>
+      <c r="AD76" s="104"/>
+      <c r="AE76" s="104"/>
+      <c r="AF76" s="104"/>
+      <c r="AG76" s="104"/>
+      <c r="AH76" s="104"/>
+      <c r="AI76" s="104"/>
+      <c r="AJ76" s="104"/>
+      <c r="AK76" s="104"/>
+      <c r="AL76" s="104"/>
+      <c r="AM76" s="104"/>
+      <c r="AN76" s="104"/>
+      <c r="AO76" s="104"/>
+      <c r="AP76" s="104"/>
+      <c r="AQ76" s="104"/>
+      <c r="AR76" s="104"/>
+      <c r="AS76" s="104"/>
+      <c r="AT76" s="104"/>
+      <c r="AU76" s="104"/>
+      <c r="AV76" s="104"/>
+      <c r="AW76" s="104"/>
+      <c r="AX76" s="104"/>
+      <c r="AY76" s="104"/>
+      <c r="AZ76" s="104"/>
+      <c r="BA76" s="104"/>
+      <c r="BB76" s="104"/>
+      <c r="BC76" s="104"/>
+      <c r="BD76" s="104"/>
+      <c r="BE76" s="104"/>
+      <c r="BF76" s="104"/>
+      <c r="BG76" s="104"/>
+      <c r="BH76" s="104"/>
+      <c r="BI76" s="104"/>
+      <c r="BJ76" s="104"/>
+      <c r="BK76" s="104"/>
+      <c r="BL76" s="104"/>
+      <c r="BM76" s="104"/>
+      <c r="BN76" s="104"/>
+      <c r="BO76" s="104"/>
+      <c r="BP76" s="105"/>
       <c r="BQ76" s="38"/>
     </row>
     <row r="77" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A77" s="87"/>
-      <c r="B77" s="87"/>
-      <c r="C77" s="87"/>
-      <c r="D77" s="87"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="87"/>
-      <c r="G77" s="87"/>
-      <c r="H77" s="87"/>
-      <c r="I77" s="87"/>
-      <c r="J77" s="87"/>
-      <c r="K77" s="87"/>
-      <c r="L77" s="87"/>
-      <c r="M77" s="87"/>
-      <c r="N77" s="87"/>
-      <c r="O77" s="87"/>
-      <c r="P77" s="87"/>
-      <c r="Q77" s="87"/>
-      <c r="R77" s="87"/>
-      <c r="S77" s="87"/>
-      <c r="T77" s="87"/>
-      <c r="U77" s="87"/>
-      <c r="V77" s="87"/>
-      <c r="W77" s="87"/>
-      <c r="X77" s="87"/>
-      <c r="Y77" s="87"/>
-      <c r="Z77" s="87"/>
-      <c r="AA77" s="87"/>
-      <c r="AB77" s="87"/>
-      <c r="AC77" s="87"/>
-      <c r="AD77" s="87"/>
-      <c r="AE77" s="87"/>
-      <c r="AF77" s="87"/>
-      <c r="AG77" s="87"/>
-      <c r="AH77" s="87"/>
-      <c r="AI77" s="87"/>
-      <c r="AJ77" s="87"/>
-      <c r="AK77" s="87"/>
-      <c r="AL77" s="87"/>
-      <c r="AM77" s="87"/>
-      <c r="AN77" s="87"/>
-      <c r="AO77" s="87"/>
-      <c r="AP77" s="87"/>
-      <c r="AQ77" s="87"/>
-      <c r="AR77" s="87"/>
-      <c r="AS77" s="87"/>
-      <c r="AT77" s="87"/>
-      <c r="AU77" s="87"/>
-      <c r="AV77" s="87"/>
-      <c r="AW77" s="87"/>
-      <c r="AX77" s="87"/>
-      <c r="AY77" s="87"/>
-      <c r="AZ77" s="87"/>
-      <c r="BA77" s="87"/>
-      <c r="BB77" s="87"/>
-      <c r="BC77" s="87"/>
-      <c r="BD77" s="87"/>
-      <c r="BE77" s="87"/>
-      <c r="BF77" s="87"/>
-      <c r="BG77" s="87"/>
-      <c r="BH77" s="87"/>
-      <c r="BI77" s="87"/>
-      <c r="BJ77" s="87"/>
-      <c r="BK77" s="87"/>
-      <c r="BL77" s="87"/>
-      <c r="BM77" s="87"/>
-      <c r="BN77" s="87"/>
-      <c r="BO77" s="87"/>
-      <c r="BP77" s="88"/>
+      <c r="A77" s="104"/>
+      <c r="B77" s="104"/>
+      <c r="C77" s="104"/>
+      <c r="D77" s="104"/>
+      <c r="E77" s="104"/>
+      <c r="F77" s="104"/>
+      <c r="G77" s="104"/>
+      <c r="H77" s="104"/>
+      <c r="I77" s="104"/>
+      <c r="J77" s="104"/>
+      <c r="K77" s="104"/>
+      <c r="L77" s="104"/>
+      <c r="M77" s="104"/>
+      <c r="N77" s="104"/>
+      <c r="O77" s="104"/>
+      <c r="P77" s="104"/>
+      <c r="Q77" s="104"/>
+      <c r="R77" s="104"/>
+      <c r="S77" s="104"/>
+      <c r="T77" s="104"/>
+      <c r="U77" s="104"/>
+      <c r="V77" s="104"/>
+      <c r="W77" s="104"/>
+      <c r="X77" s="104"/>
+      <c r="Y77" s="104"/>
+      <c r="Z77" s="104"/>
+      <c r="AA77" s="104"/>
+      <c r="AB77" s="104"/>
+      <c r="AC77" s="104"/>
+      <c r="AD77" s="104"/>
+      <c r="AE77" s="104"/>
+      <c r="AF77" s="104"/>
+      <c r="AG77" s="104"/>
+      <c r="AH77" s="104"/>
+      <c r="AI77" s="104"/>
+      <c r="AJ77" s="104"/>
+      <c r="AK77" s="104"/>
+      <c r="AL77" s="104"/>
+      <c r="AM77" s="104"/>
+      <c r="AN77" s="104"/>
+      <c r="AO77" s="104"/>
+      <c r="AP77" s="104"/>
+      <c r="AQ77" s="104"/>
+      <c r="AR77" s="104"/>
+      <c r="AS77" s="104"/>
+      <c r="AT77" s="104"/>
+      <c r="AU77" s="104"/>
+      <c r="AV77" s="104"/>
+      <c r="AW77" s="104"/>
+      <c r="AX77" s="104"/>
+      <c r="AY77" s="104"/>
+      <c r="AZ77" s="104"/>
+      <c r="BA77" s="104"/>
+      <c r="BB77" s="104"/>
+      <c r="BC77" s="104"/>
+      <c r="BD77" s="104"/>
+      <c r="BE77" s="104"/>
+      <c r="BF77" s="104"/>
+      <c r="BG77" s="104"/>
+      <c r="BH77" s="104"/>
+      <c r="BI77" s="104"/>
+      <c r="BJ77" s="104"/>
+      <c r="BK77" s="104"/>
+      <c r="BL77" s="104"/>
+      <c r="BM77" s="104"/>
+      <c r="BN77" s="104"/>
+      <c r="BO77" s="104"/>
+      <c r="BP77" s="105"/>
       <c r="BQ77" s="38"/>
     </row>
     <row r="78" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A78" s="87"/>
-      <c r="B78" s="87"/>
-      <c r="C78" s="87"/>
-      <c r="D78" s="87"/>
-      <c r="E78" s="87"/>
-      <c r="F78" s="87"/>
-      <c r="G78" s="87"/>
-      <c r="H78" s="87"/>
-      <c r="I78" s="87"/>
-      <c r="J78" s="87"/>
-      <c r="K78" s="87"/>
-      <c r="L78" s="87"/>
-      <c r="M78" s="87"/>
-      <c r="N78" s="87"/>
-      <c r="O78" s="87"/>
-      <c r="P78" s="87"/>
-      <c r="Q78" s="87"/>
-      <c r="R78" s="87"/>
-      <c r="S78" s="87"/>
-      <c r="T78" s="87"/>
-      <c r="U78" s="87"/>
-      <c r="V78" s="87"/>
-      <c r="W78" s="87"/>
-      <c r="X78" s="87"/>
-      <c r="Y78" s="87"/>
-      <c r="Z78" s="87"/>
-      <c r="AA78" s="87"/>
-      <c r="AB78" s="87"/>
-      <c r="AC78" s="87"/>
-      <c r="AD78" s="87"/>
-      <c r="AE78" s="87"/>
-      <c r="AF78" s="87"/>
-      <c r="AG78" s="87"/>
-      <c r="AH78" s="87"/>
-      <c r="AI78" s="87"/>
-      <c r="AJ78" s="87"/>
-      <c r="AK78" s="87"/>
-      <c r="AL78" s="87"/>
-      <c r="AM78" s="87"/>
-      <c r="AN78" s="87"/>
-      <c r="AO78" s="87"/>
-      <c r="AP78" s="87"/>
-      <c r="AQ78" s="87"/>
-      <c r="AR78" s="87"/>
-      <c r="AS78" s="87"/>
-      <c r="AT78" s="87"/>
-      <c r="AU78" s="87"/>
-      <c r="AV78" s="87"/>
-      <c r="AW78" s="87"/>
-      <c r="AX78" s="87"/>
-      <c r="AY78" s="87"/>
-      <c r="AZ78" s="87"/>
-      <c r="BA78" s="87"/>
-      <c r="BB78" s="87"/>
-      <c r="BC78" s="87"/>
-      <c r="BD78" s="87"/>
-      <c r="BE78" s="87"/>
-      <c r="BF78" s="87"/>
-      <c r="BG78" s="87"/>
-      <c r="BH78" s="87"/>
-      <c r="BI78" s="87"/>
-      <c r="BJ78" s="87"/>
-      <c r="BK78" s="87"/>
-      <c r="BL78" s="87"/>
-      <c r="BM78" s="87"/>
-      <c r="BN78" s="87"/>
-      <c r="BO78" s="87"/>
-      <c r="BP78" s="88"/>
+      <c r="A78" s="104"/>
+      <c r="B78" s="104"/>
+      <c r="C78" s="104"/>
+      <c r="D78" s="104"/>
+      <c r="E78" s="104"/>
+      <c r="F78" s="104"/>
+      <c r="G78" s="104"/>
+      <c r="H78" s="104"/>
+      <c r="I78" s="104"/>
+      <c r="J78" s="104"/>
+      <c r="K78" s="104"/>
+      <c r="L78" s="104"/>
+      <c r="M78" s="104"/>
+      <c r="N78" s="104"/>
+      <c r="O78" s="104"/>
+      <c r="P78" s="104"/>
+      <c r="Q78" s="104"/>
+      <c r="R78" s="104"/>
+      <c r="S78" s="104"/>
+      <c r="T78" s="104"/>
+      <c r="U78" s="104"/>
+      <c r="V78" s="104"/>
+      <c r="W78" s="104"/>
+      <c r="X78" s="104"/>
+      <c r="Y78" s="104"/>
+      <c r="Z78" s="104"/>
+      <c r="AA78" s="104"/>
+      <c r="AB78" s="104"/>
+      <c r="AC78" s="104"/>
+      <c r="AD78" s="104"/>
+      <c r="AE78" s="104"/>
+      <c r="AF78" s="104"/>
+      <c r="AG78" s="104"/>
+      <c r="AH78" s="104"/>
+      <c r="AI78" s="104"/>
+      <c r="AJ78" s="104"/>
+      <c r="AK78" s="104"/>
+      <c r="AL78" s="104"/>
+      <c r="AM78" s="104"/>
+      <c r="AN78" s="104"/>
+      <c r="AO78" s="104"/>
+      <c r="AP78" s="104"/>
+      <c r="AQ78" s="104"/>
+      <c r="AR78" s="104"/>
+      <c r="AS78" s="104"/>
+      <c r="AT78" s="104"/>
+      <c r="AU78" s="104"/>
+      <c r="AV78" s="104"/>
+      <c r="AW78" s="104"/>
+      <c r="AX78" s="104"/>
+      <c r="AY78" s="104"/>
+      <c r="AZ78" s="104"/>
+      <c r="BA78" s="104"/>
+      <c r="BB78" s="104"/>
+      <c r="BC78" s="104"/>
+      <c r="BD78" s="104"/>
+      <c r="BE78" s="104"/>
+      <c r="BF78" s="104"/>
+      <c r="BG78" s="104"/>
+      <c r="BH78" s="104"/>
+      <c r="BI78" s="104"/>
+      <c r="BJ78" s="104"/>
+      <c r="BK78" s="104"/>
+      <c r="BL78" s="104"/>
+      <c r="BM78" s="104"/>
+      <c r="BN78" s="104"/>
+      <c r="BO78" s="104"/>
+      <c r="BP78" s="105"/>
       <c r="BQ78" s="38"/>
     </row>
     <row r="79" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A79" s="87"/>
-      <c r="B79" s="87"/>
-      <c r="C79" s="87"/>
-      <c r="D79" s="87"/>
-      <c r="E79" s="87"/>
-      <c r="F79" s="87"/>
-      <c r="G79" s="87"/>
-      <c r="H79" s="87"/>
-      <c r="I79" s="87"/>
-      <c r="J79" s="87"/>
-      <c r="K79" s="87"/>
-      <c r="L79" s="87"/>
-      <c r="M79" s="87"/>
-      <c r="N79" s="87"/>
-      <c r="O79" s="87"/>
-      <c r="P79" s="87"/>
-      <c r="Q79" s="87"/>
-      <c r="R79" s="87"/>
-      <c r="S79" s="87"/>
-      <c r="T79" s="87"/>
-      <c r="U79" s="87"/>
-      <c r="V79" s="87"/>
-      <c r="W79" s="87"/>
-      <c r="X79" s="87"/>
-      <c r="Y79" s="87"/>
-      <c r="Z79" s="87"/>
-      <c r="AA79" s="87"/>
-      <c r="AB79" s="87"/>
-      <c r="AC79" s="87"/>
-      <c r="AD79" s="87"/>
-      <c r="AE79" s="87"/>
-      <c r="AF79" s="87"/>
-      <c r="AG79" s="87"/>
-      <c r="AH79" s="87"/>
-      <c r="AI79" s="87"/>
-      <c r="AJ79" s="87"/>
-      <c r="AK79" s="87"/>
-      <c r="AL79" s="87"/>
-      <c r="AM79" s="87"/>
-      <c r="AN79" s="87"/>
-      <c r="AO79" s="87"/>
-      <c r="AP79" s="87"/>
-      <c r="AQ79" s="87"/>
-      <c r="AR79" s="87"/>
-      <c r="AS79" s="87"/>
-      <c r="AT79" s="87"/>
-      <c r="AU79" s="87"/>
-      <c r="AV79" s="87"/>
-      <c r="AW79" s="87"/>
-      <c r="AX79" s="87"/>
-      <c r="AY79" s="87"/>
-      <c r="AZ79" s="87"/>
-      <c r="BA79" s="87"/>
-      <c r="BB79" s="87"/>
-      <c r="BC79" s="87"/>
-      <c r="BD79" s="87"/>
-      <c r="BE79" s="87"/>
-      <c r="BF79" s="87"/>
-      <c r="BG79" s="87"/>
-      <c r="BH79" s="87"/>
-      <c r="BI79" s="87"/>
-      <c r="BJ79" s="87"/>
-      <c r="BK79" s="87"/>
-      <c r="BL79" s="87"/>
-      <c r="BM79" s="87"/>
-      <c r="BN79" s="87"/>
-      <c r="BO79" s="87"/>
-      <c r="BP79" s="88"/>
+      <c r="A79" s="104"/>
+      <c r="B79" s="104"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="104"/>
+      <c r="E79" s="104"/>
+      <c r="F79" s="104"/>
+      <c r="G79" s="104"/>
+      <c r="H79" s="104"/>
+      <c r="I79" s="104"/>
+      <c r="J79" s="104"/>
+      <c r="K79" s="104"/>
+      <c r="L79" s="104"/>
+      <c r="M79" s="104"/>
+      <c r="N79" s="104"/>
+      <c r="O79" s="104"/>
+      <c r="P79" s="104"/>
+      <c r="Q79" s="104"/>
+      <c r="R79" s="104"/>
+      <c r="S79" s="104"/>
+      <c r="T79" s="104"/>
+      <c r="U79" s="104"/>
+      <c r="V79" s="104"/>
+      <c r="W79" s="104"/>
+      <c r="X79" s="104"/>
+      <c r="Y79" s="104"/>
+      <c r="Z79" s="104"/>
+      <c r="AA79" s="104"/>
+      <c r="AB79" s="104"/>
+      <c r="AC79" s="104"/>
+      <c r="AD79" s="104"/>
+      <c r="AE79" s="104"/>
+      <c r="AF79" s="104"/>
+      <c r="AG79" s="104"/>
+      <c r="AH79" s="104"/>
+      <c r="AI79" s="104"/>
+      <c r="AJ79" s="104"/>
+      <c r="AK79" s="104"/>
+      <c r="AL79" s="104"/>
+      <c r="AM79" s="104"/>
+      <c r="AN79" s="104"/>
+      <c r="AO79" s="104"/>
+      <c r="AP79" s="104"/>
+      <c r="AQ79" s="104"/>
+      <c r="AR79" s="104"/>
+      <c r="AS79" s="104"/>
+      <c r="AT79" s="104"/>
+      <c r="AU79" s="104"/>
+      <c r="AV79" s="104"/>
+      <c r="AW79" s="104"/>
+      <c r="AX79" s="104"/>
+      <c r="AY79" s="104"/>
+      <c r="AZ79" s="104"/>
+      <c r="BA79" s="104"/>
+      <c r="BB79" s="104"/>
+      <c r="BC79" s="104"/>
+      <c r="BD79" s="104"/>
+      <c r="BE79" s="104"/>
+      <c r="BF79" s="104"/>
+      <c r="BG79" s="104"/>
+      <c r="BH79" s="104"/>
+      <c r="BI79" s="104"/>
+      <c r="BJ79" s="104"/>
+      <c r="BK79" s="104"/>
+      <c r="BL79" s="104"/>
+      <c r="BM79" s="104"/>
+      <c r="BN79" s="104"/>
+      <c r="BO79" s="104"/>
+      <c r="BP79" s="105"/>
       <c r="BQ79" s="38"/>
     </row>
     <row r="80" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A80" s="87"/>
-      <c r="B80" s="87"/>
-      <c r="C80" s="87"/>
-      <c r="D80" s="87"/>
-      <c r="E80" s="87"/>
-      <c r="F80" s="87"/>
-      <c r="G80" s="87"/>
-      <c r="H80" s="87"/>
-      <c r="I80" s="87"/>
-      <c r="J80" s="87"/>
-      <c r="K80" s="87"/>
-      <c r="L80" s="87"/>
-      <c r="M80" s="87"/>
-      <c r="N80" s="87"/>
-      <c r="O80" s="87"/>
-      <c r="P80" s="87"/>
-      <c r="Q80" s="87"/>
-      <c r="R80" s="87"/>
-      <c r="S80" s="87"/>
-      <c r="T80" s="87"/>
-      <c r="U80" s="87"/>
-      <c r="V80" s="87"/>
-      <c r="W80" s="87"/>
-      <c r="X80" s="87"/>
-      <c r="Y80" s="87"/>
-      <c r="Z80" s="87"/>
-      <c r="AA80" s="87"/>
-      <c r="AB80" s="87"/>
-      <c r="AC80" s="87"/>
-      <c r="AD80" s="87"/>
-      <c r="AE80" s="87"/>
-      <c r="AF80" s="87"/>
-      <c r="AG80" s="87"/>
-      <c r="AH80" s="87"/>
-      <c r="AI80" s="87"/>
-      <c r="AJ80" s="87"/>
-      <c r="AK80" s="87"/>
-      <c r="AL80" s="87"/>
-      <c r="AM80" s="87"/>
-      <c r="AN80" s="87"/>
-      <c r="AO80" s="87"/>
-      <c r="AP80" s="87"/>
-      <c r="AQ80" s="87"/>
-      <c r="AR80" s="87"/>
-      <c r="AS80" s="87"/>
-      <c r="AT80" s="87"/>
-      <c r="AU80" s="87"/>
-      <c r="AV80" s="87"/>
-      <c r="AW80" s="87"/>
-      <c r="AX80" s="87"/>
-      <c r="AY80" s="87"/>
-      <c r="AZ80" s="87"/>
-      <c r="BA80" s="87"/>
-      <c r="BB80" s="87"/>
-      <c r="BC80" s="87"/>
-      <c r="BD80" s="87"/>
-      <c r="BE80" s="87"/>
-      <c r="BF80" s="87"/>
-      <c r="BG80" s="87"/>
-      <c r="BH80" s="87"/>
-      <c r="BI80" s="87"/>
-      <c r="BJ80" s="87"/>
-      <c r="BK80" s="87"/>
-      <c r="BL80" s="87"/>
-      <c r="BM80" s="87"/>
-      <c r="BN80" s="87"/>
-      <c r="BO80" s="87"/>
-      <c r="BP80" s="88"/>
+      <c r="A80" s="104"/>
+      <c r="B80" s="104"/>
+      <c r="C80" s="104"/>
+      <c r="D80" s="104"/>
+      <c r="E80" s="104"/>
+      <c r="F80" s="104"/>
+      <c r="G80" s="104"/>
+      <c r="H80" s="104"/>
+      <c r="I80" s="104"/>
+      <c r="J80" s="104"/>
+      <c r="K80" s="104"/>
+      <c r="L80" s="104"/>
+      <c r="M80" s="104"/>
+      <c r="N80" s="104"/>
+      <c r="O80" s="104"/>
+      <c r="P80" s="104"/>
+      <c r="Q80" s="104"/>
+      <c r="R80" s="104"/>
+      <c r="S80" s="104"/>
+      <c r="T80" s="104"/>
+      <c r="U80" s="104"/>
+      <c r="V80" s="104"/>
+      <c r="W80" s="104"/>
+      <c r="X80" s="104"/>
+      <c r="Y80" s="104"/>
+      <c r="Z80" s="104"/>
+      <c r="AA80" s="104"/>
+      <c r="AB80" s="104"/>
+      <c r="AC80" s="104"/>
+      <c r="AD80" s="104"/>
+      <c r="AE80" s="104"/>
+      <c r="AF80" s="104"/>
+      <c r="AG80" s="104"/>
+      <c r="AH80" s="104"/>
+      <c r="AI80" s="104"/>
+      <c r="AJ80" s="104"/>
+      <c r="AK80" s="104"/>
+      <c r="AL80" s="104"/>
+      <c r="AM80" s="104"/>
+      <c r="AN80" s="104"/>
+      <c r="AO80" s="104"/>
+      <c r="AP80" s="104"/>
+      <c r="AQ80" s="104"/>
+      <c r="AR80" s="104"/>
+      <c r="AS80" s="104"/>
+      <c r="AT80" s="104"/>
+      <c r="AU80" s="104"/>
+      <c r="AV80" s="104"/>
+      <c r="AW80" s="104"/>
+      <c r="AX80" s="104"/>
+      <c r="AY80" s="104"/>
+      <c r="AZ80" s="104"/>
+      <c r="BA80" s="104"/>
+      <c r="BB80" s="104"/>
+      <c r="BC80" s="104"/>
+      <c r="BD80" s="104"/>
+      <c r="BE80" s="104"/>
+      <c r="BF80" s="104"/>
+      <c r="BG80" s="104"/>
+      <c r="BH80" s="104"/>
+      <c r="BI80" s="104"/>
+      <c r="BJ80" s="104"/>
+      <c r="BK80" s="104"/>
+      <c r="BL80" s="104"/>
+      <c r="BM80" s="104"/>
+      <c r="BN80" s="104"/>
+      <c r="BO80" s="104"/>
+      <c r="BP80" s="105"/>
       <c r="BQ80" s="38"/>
     </row>
     <row r="81" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A81" s="87"/>
-      <c r="B81" s="87"/>
-      <c r="C81" s="87"/>
-      <c r="D81" s="87"/>
-      <c r="E81" s="87"/>
-      <c r="F81" s="87"/>
-      <c r="G81" s="87"/>
-      <c r="H81" s="87"/>
-      <c r="I81" s="87"/>
-      <c r="J81" s="87"/>
-      <c r="K81" s="87"/>
-      <c r="L81" s="87"/>
-      <c r="M81" s="87"/>
-      <c r="N81" s="87"/>
-      <c r="O81" s="87"/>
-      <c r="P81" s="87"/>
-      <c r="Q81" s="87"/>
-      <c r="R81" s="87"/>
-      <c r="S81" s="87"/>
-      <c r="T81" s="87"/>
-      <c r="U81" s="87"/>
-      <c r="V81" s="87"/>
-      <c r="W81" s="87"/>
-      <c r="X81" s="87"/>
-      <c r="Y81" s="87"/>
-      <c r="Z81" s="87"/>
-      <c r="AA81" s="87"/>
-      <c r="AB81" s="87"/>
-      <c r="AC81" s="87"/>
-      <c r="AD81" s="87"/>
-      <c r="AE81" s="87"/>
-      <c r="AF81" s="87"/>
-      <c r="AG81" s="87"/>
-      <c r="AH81" s="87"/>
-      <c r="AI81" s="87"/>
-      <c r="AJ81" s="87"/>
-      <c r="AK81" s="87"/>
-      <c r="AL81" s="87"/>
-      <c r="AM81" s="87"/>
-      <c r="AN81" s="87"/>
-      <c r="AO81" s="87"/>
-      <c r="AP81" s="87"/>
-      <c r="AQ81" s="87"/>
-      <c r="AR81" s="87"/>
-      <c r="AS81" s="87"/>
-      <c r="AT81" s="87"/>
-      <c r="AU81" s="87"/>
-      <c r="AV81" s="87"/>
-      <c r="AW81" s="87"/>
-      <c r="AX81" s="87"/>
-      <c r="AY81" s="87"/>
-      <c r="AZ81" s="87"/>
-      <c r="BA81" s="87"/>
-      <c r="BB81" s="87"/>
-      <c r="BC81" s="87"/>
-      <c r="BD81" s="87"/>
-      <c r="BE81" s="87"/>
-      <c r="BF81" s="87"/>
-      <c r="BG81" s="87"/>
-      <c r="BH81" s="87"/>
-      <c r="BI81" s="87"/>
-      <c r="BJ81" s="87"/>
-      <c r="BK81" s="87"/>
-      <c r="BL81" s="87"/>
-      <c r="BM81" s="87"/>
-      <c r="BN81" s="87"/>
-      <c r="BO81" s="87"/>
-      <c r="BP81" s="88"/>
+      <c r="A81" s="104"/>
+      <c r="B81" s="104"/>
+      <c r="C81" s="104"/>
+      <c r="D81" s="104"/>
+      <c r="E81" s="104"/>
+      <c r="F81" s="104"/>
+      <c r="G81" s="104"/>
+      <c r="H81" s="104"/>
+      <c r="I81" s="104"/>
+      <c r="J81" s="104"/>
+      <c r="K81" s="104"/>
+      <c r="L81" s="104"/>
+      <c r="M81" s="104"/>
+      <c r="N81" s="104"/>
+      <c r="O81" s="104"/>
+      <c r="P81" s="104"/>
+      <c r="Q81" s="104"/>
+      <c r="R81" s="104"/>
+      <c r="S81" s="104"/>
+      <c r="T81" s="104"/>
+      <c r="U81" s="104"/>
+      <c r="V81" s="104"/>
+      <c r="W81" s="104"/>
+      <c r="X81" s="104"/>
+      <c r="Y81" s="104"/>
+      <c r="Z81" s="104"/>
+      <c r="AA81" s="104"/>
+      <c r="AB81" s="104"/>
+      <c r="AC81" s="104"/>
+      <c r="AD81" s="104"/>
+      <c r="AE81" s="104"/>
+      <c r="AF81" s="104"/>
+      <c r="AG81" s="104"/>
+      <c r="AH81" s="104"/>
+      <c r="AI81" s="104"/>
+      <c r="AJ81" s="104"/>
+      <c r="AK81" s="104"/>
+      <c r="AL81" s="104"/>
+      <c r="AM81" s="104"/>
+      <c r="AN81" s="104"/>
+      <c r="AO81" s="104"/>
+      <c r="AP81" s="104"/>
+      <c r="AQ81" s="104"/>
+      <c r="AR81" s="104"/>
+      <c r="AS81" s="104"/>
+      <c r="AT81" s="104"/>
+      <c r="AU81" s="104"/>
+      <c r="AV81" s="104"/>
+      <c r="AW81" s="104"/>
+      <c r="AX81" s="104"/>
+      <c r="AY81" s="104"/>
+      <c r="AZ81" s="104"/>
+      <c r="BA81" s="104"/>
+      <c r="BB81" s="104"/>
+      <c r="BC81" s="104"/>
+      <c r="BD81" s="104"/>
+      <c r="BE81" s="104"/>
+      <c r="BF81" s="104"/>
+      <c r="BG81" s="104"/>
+      <c r="BH81" s="104"/>
+      <c r="BI81" s="104"/>
+      <c r="BJ81" s="104"/>
+      <c r="BK81" s="104"/>
+      <c r="BL81" s="104"/>
+      <c r="BM81" s="104"/>
+      <c r="BN81" s="104"/>
+      <c r="BO81" s="104"/>
+      <c r="BP81" s="105"/>
       <c r="BQ81" s="38"/>
     </row>
     <row r="82" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A82" s="87"/>
-      <c r="B82" s="87"/>
-      <c r="C82" s="87"/>
-      <c r="D82" s="87"/>
-      <c r="E82" s="87"/>
-      <c r="F82" s="87"/>
-      <c r="G82" s="87"/>
-      <c r="H82" s="87"/>
-      <c r="I82" s="87"/>
-      <c r="J82" s="87"/>
-      <c r="K82" s="87"/>
-      <c r="L82" s="87"/>
-      <c r="M82" s="87"/>
-      <c r="N82" s="87"/>
-      <c r="O82" s="87"/>
-      <c r="P82" s="87"/>
-      <c r="Q82" s="87"/>
-      <c r="R82" s="87"/>
-      <c r="S82" s="87"/>
-      <c r="T82" s="87"/>
-      <c r="U82" s="87"/>
-      <c r="V82" s="87"/>
-      <c r="W82" s="87"/>
-      <c r="X82" s="87"/>
-      <c r="Y82" s="87"/>
-      <c r="Z82" s="87"/>
-      <c r="AA82" s="87"/>
-      <c r="AB82" s="87"/>
-      <c r="AC82" s="87"/>
-      <c r="AD82" s="87"/>
-      <c r="AE82" s="87"/>
-      <c r="AF82" s="87"/>
-      <c r="AG82" s="87"/>
-      <c r="AH82" s="87"/>
-      <c r="AI82" s="87"/>
-      <c r="AJ82" s="87"/>
-      <c r="AK82" s="87"/>
-      <c r="AL82" s="87"/>
-      <c r="AM82" s="87"/>
-      <c r="AN82" s="87"/>
-      <c r="AO82" s="87"/>
-      <c r="AP82" s="87"/>
-      <c r="AQ82" s="87"/>
-      <c r="AR82" s="87"/>
-      <c r="AS82" s="87"/>
-      <c r="AT82" s="87"/>
-      <c r="AU82" s="87"/>
-      <c r="AV82" s="87"/>
-      <c r="AW82" s="87"/>
-      <c r="AX82" s="87"/>
-      <c r="AY82" s="87"/>
-      <c r="AZ82" s="87"/>
-      <c r="BA82" s="87"/>
-      <c r="BB82" s="87"/>
-      <c r="BC82" s="87"/>
-      <c r="BD82" s="87"/>
-      <c r="BE82" s="87"/>
-      <c r="BF82" s="87"/>
-      <c r="BG82" s="87"/>
-      <c r="BH82" s="87"/>
-      <c r="BI82" s="87"/>
-      <c r="BJ82" s="87"/>
-      <c r="BK82" s="87"/>
-      <c r="BL82" s="87"/>
-      <c r="BM82" s="87"/>
-      <c r="BN82" s="87"/>
-      <c r="BO82" s="87"/>
-      <c r="BP82" s="88"/>
+      <c r="A82" s="104"/>
+      <c r="B82" s="104"/>
+      <c r="C82" s="104"/>
+      <c r="D82" s="104"/>
+      <c r="E82" s="104"/>
+      <c r="F82" s="104"/>
+      <c r="G82" s="104"/>
+      <c r="H82" s="104"/>
+      <c r="I82" s="104"/>
+      <c r="J82" s="104"/>
+      <c r="K82" s="104"/>
+      <c r="L82" s="104"/>
+      <c r="M82" s="104"/>
+      <c r="N82" s="104"/>
+      <c r="O82" s="104"/>
+      <c r="P82" s="104"/>
+      <c r="Q82" s="104"/>
+      <c r="R82" s="104"/>
+      <c r="S82" s="104"/>
+      <c r="T82" s="104"/>
+      <c r="U82" s="104"/>
+      <c r="V82" s="104"/>
+      <c r="W82" s="104"/>
+      <c r="X82" s="104"/>
+      <c r="Y82" s="104"/>
+      <c r="Z82" s="104"/>
+      <c r="AA82" s="104"/>
+      <c r="AB82" s="104"/>
+      <c r="AC82" s="104"/>
+      <c r="AD82" s="104"/>
+      <c r="AE82" s="104"/>
+      <c r="AF82" s="104"/>
+      <c r="AG82" s="104"/>
+      <c r="AH82" s="104"/>
+      <c r="AI82" s="104"/>
+      <c r="AJ82" s="104"/>
+      <c r="AK82" s="104"/>
+      <c r="AL82" s="104"/>
+      <c r="AM82" s="104"/>
+      <c r="AN82" s="104"/>
+      <c r="AO82" s="104"/>
+      <c r="AP82" s="104"/>
+      <c r="AQ82" s="104"/>
+      <c r="AR82" s="104"/>
+      <c r="AS82" s="104"/>
+      <c r="AT82" s="104"/>
+      <c r="AU82" s="104"/>
+      <c r="AV82" s="104"/>
+      <c r="AW82" s="104"/>
+      <c r="AX82" s="104"/>
+      <c r="AY82" s="104"/>
+      <c r="AZ82" s="104"/>
+      <c r="BA82" s="104"/>
+      <c r="BB82" s="104"/>
+      <c r="BC82" s="104"/>
+      <c r="BD82" s="104"/>
+      <c r="BE82" s="104"/>
+      <c r="BF82" s="104"/>
+      <c r="BG82" s="104"/>
+      <c r="BH82" s="104"/>
+      <c r="BI82" s="104"/>
+      <c r="BJ82" s="104"/>
+      <c r="BK82" s="104"/>
+      <c r="BL82" s="104"/>
+      <c r="BM82" s="104"/>
+      <c r="BN82" s="104"/>
+      <c r="BO82" s="104"/>
+      <c r="BP82" s="105"/>
       <c r="BQ82" s="38"/>
     </row>
     <row r="83" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A83" s="87"/>
-      <c r="B83" s="87"/>
-      <c r="C83" s="87"/>
-      <c r="D83" s="87"/>
-      <c r="E83" s="87"/>
-      <c r="F83" s="87"/>
-      <c r="G83" s="87"/>
-      <c r="H83" s="87"/>
-      <c r="I83" s="87"/>
-      <c r="J83" s="87"/>
-      <c r="K83" s="87"/>
-      <c r="L83" s="87"/>
-      <c r="M83" s="87"/>
-      <c r="N83" s="87"/>
-      <c r="O83" s="87"/>
-      <c r="P83" s="87"/>
-      <c r="Q83" s="87"/>
-      <c r="R83" s="87"/>
-      <c r="S83" s="87"/>
-      <c r="T83" s="87"/>
-      <c r="U83" s="87"/>
-      <c r="V83" s="87"/>
-      <c r="W83" s="87"/>
-      <c r="X83" s="87"/>
-      <c r="Y83" s="87"/>
-      <c r="Z83" s="87"/>
-      <c r="AA83" s="87"/>
-      <c r="AB83" s="87"/>
-      <c r="AC83" s="87"/>
-      <c r="AD83" s="87"/>
-      <c r="AE83" s="87"/>
-      <c r="AF83" s="87"/>
-      <c r="AG83" s="87"/>
-      <c r="AH83" s="87"/>
-      <c r="AI83" s="87"/>
-      <c r="AJ83" s="87"/>
-      <c r="AK83" s="87"/>
-      <c r="AL83" s="87"/>
-      <c r="AM83" s="87"/>
-      <c r="AN83" s="87"/>
-      <c r="AO83" s="87"/>
-      <c r="AP83" s="87"/>
-      <c r="AQ83" s="87"/>
-      <c r="AR83" s="87"/>
-      <c r="AS83" s="87"/>
-      <c r="AT83" s="87"/>
-      <c r="AU83" s="87"/>
-      <c r="AV83" s="87"/>
-      <c r="AW83" s="87"/>
-      <c r="AX83" s="87"/>
-      <c r="AY83" s="87"/>
-      <c r="AZ83" s="87"/>
-      <c r="BA83" s="87"/>
-      <c r="BB83" s="87"/>
-      <c r="BC83" s="87"/>
-      <c r="BD83" s="87"/>
-      <c r="BE83" s="87"/>
-      <c r="BF83" s="87"/>
-      <c r="BG83" s="87"/>
-      <c r="BH83" s="87"/>
-      <c r="BI83" s="87"/>
-      <c r="BJ83" s="87"/>
-      <c r="BK83" s="87"/>
-      <c r="BL83" s="87"/>
-      <c r="BM83" s="87"/>
-      <c r="BN83" s="87"/>
-      <c r="BO83" s="87"/>
-      <c r="BP83" s="88"/>
+      <c r="A83" s="104"/>
+      <c r="B83" s="104"/>
+      <c r="C83" s="104"/>
+      <c r="D83" s="104"/>
+      <c r="E83" s="104"/>
+      <c r="F83" s="104"/>
+      <c r="G83" s="104"/>
+      <c r="H83" s="104"/>
+      <c r="I83" s="104"/>
+      <c r="J83" s="104"/>
+      <c r="K83" s="104"/>
+      <c r="L83" s="104"/>
+      <c r="M83" s="104"/>
+      <c r="N83" s="104"/>
+      <c r="O83" s="104"/>
+      <c r="P83" s="104"/>
+      <c r="Q83" s="104"/>
+      <c r="R83" s="104"/>
+      <c r="S83" s="104"/>
+      <c r="T83" s="104"/>
+      <c r="U83" s="104"/>
+      <c r="V83" s="104"/>
+      <c r="W83" s="104"/>
+      <c r="X83" s="104"/>
+      <c r="Y83" s="104"/>
+      <c r="Z83" s="104"/>
+      <c r="AA83" s="104"/>
+      <c r="AB83" s="104"/>
+      <c r="AC83" s="104"/>
+      <c r="AD83" s="104"/>
+      <c r="AE83" s="104"/>
+      <c r="AF83" s="104"/>
+      <c r="AG83" s="104"/>
+      <c r="AH83" s="104"/>
+      <c r="AI83" s="104"/>
+      <c r="AJ83" s="104"/>
+      <c r="AK83" s="104"/>
+      <c r="AL83" s="104"/>
+      <c r="AM83" s="104"/>
+      <c r="AN83" s="104"/>
+      <c r="AO83" s="104"/>
+      <c r="AP83" s="104"/>
+      <c r="AQ83" s="104"/>
+      <c r="AR83" s="104"/>
+      <c r="AS83" s="104"/>
+      <c r="AT83" s="104"/>
+      <c r="AU83" s="104"/>
+      <c r="AV83" s="104"/>
+      <c r="AW83" s="104"/>
+      <c r="AX83" s="104"/>
+      <c r="AY83" s="104"/>
+      <c r="AZ83" s="104"/>
+      <c r="BA83" s="104"/>
+      <c r="BB83" s="104"/>
+      <c r="BC83" s="104"/>
+      <c r="BD83" s="104"/>
+      <c r="BE83" s="104"/>
+      <c r="BF83" s="104"/>
+      <c r="BG83" s="104"/>
+      <c r="BH83" s="104"/>
+      <c r="BI83" s="104"/>
+      <c r="BJ83" s="104"/>
+      <c r="BK83" s="104"/>
+      <c r="BL83" s="104"/>
+      <c r="BM83" s="104"/>
+      <c r="BN83" s="104"/>
+      <c r="BO83" s="104"/>
+      <c r="BP83" s="105"/>
       <c r="BQ83" s="38"/>
     </row>
     <row r="84" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A84" s="87"/>
-      <c r="B84" s="87"/>
-      <c r="C84" s="87"/>
-      <c r="D84" s="87"/>
-      <c r="E84" s="87"/>
-      <c r="F84" s="87"/>
-      <c r="G84" s="87"/>
-      <c r="H84" s="87"/>
-      <c r="I84" s="87"/>
-      <c r="J84" s="87"/>
-      <c r="K84" s="87"/>
-      <c r="L84" s="87"/>
-      <c r="M84" s="87"/>
-      <c r="N84" s="87"/>
-      <c r="O84" s="87"/>
-      <c r="P84" s="87"/>
-      <c r="Q84" s="87"/>
-      <c r="R84" s="87"/>
-      <c r="S84" s="87"/>
-      <c r="T84" s="87"/>
-      <c r="U84" s="87"/>
-      <c r="V84" s="87"/>
-      <c r="W84" s="87"/>
-      <c r="X84" s="87"/>
-      <c r="Y84" s="87"/>
-      <c r="Z84" s="87"/>
-      <c r="AA84" s="87"/>
-      <c r="AB84" s="87"/>
-      <c r="AC84" s="87"/>
-      <c r="AD84" s="87"/>
-      <c r="AE84" s="87"/>
-      <c r="AF84" s="87"/>
-      <c r="AG84" s="87"/>
-      <c r="AH84" s="87"/>
-      <c r="AI84" s="87"/>
-      <c r="AJ84" s="87"/>
-      <c r="AK84" s="87"/>
-      <c r="AL84" s="87"/>
-      <c r="AM84" s="87"/>
-      <c r="AN84" s="87"/>
-      <c r="AO84" s="87"/>
-      <c r="AP84" s="87"/>
-      <c r="AQ84" s="87"/>
-      <c r="AR84" s="87"/>
-      <c r="AS84" s="87"/>
-      <c r="AT84" s="87"/>
-      <c r="AU84" s="87"/>
-      <c r="AV84" s="87"/>
-      <c r="AW84" s="87"/>
-      <c r="AX84" s="87"/>
-      <c r="AY84" s="87"/>
-      <c r="AZ84" s="87"/>
-      <c r="BA84" s="87"/>
-      <c r="BB84" s="87"/>
-      <c r="BC84" s="87"/>
-      <c r="BD84" s="87"/>
-      <c r="BE84" s="87"/>
-      <c r="BF84" s="87"/>
-      <c r="BG84" s="87"/>
-      <c r="BH84" s="87"/>
-      <c r="BI84" s="87"/>
-      <c r="BJ84" s="87"/>
-      <c r="BK84" s="87"/>
-      <c r="BL84" s="87"/>
-      <c r="BM84" s="87"/>
-      <c r="BN84" s="87"/>
-      <c r="BO84" s="87"/>
-      <c r="BP84" s="88"/>
+      <c r="A84" s="104"/>
+      <c r="B84" s="104"/>
+      <c r="C84" s="104"/>
+      <c r="D84" s="104"/>
+      <c r="E84" s="104"/>
+      <c r="F84" s="104"/>
+      <c r="G84" s="104"/>
+      <c r="H84" s="104"/>
+      <c r="I84" s="104"/>
+      <c r="J84" s="104"/>
+      <c r="K84" s="104"/>
+      <c r="L84" s="104"/>
+      <c r="M84" s="104"/>
+      <c r="N84" s="104"/>
+      <c r="O84" s="104"/>
+      <c r="P84" s="104"/>
+      <c r="Q84" s="104"/>
+      <c r="R84" s="104"/>
+      <c r="S84" s="104"/>
+      <c r="T84" s="104"/>
+      <c r="U84" s="104"/>
+      <c r="V84" s="104"/>
+      <c r="W84" s="104"/>
+      <c r="X84" s="104"/>
+      <c r="Y84" s="104"/>
+      <c r="Z84" s="104"/>
+      <c r="AA84" s="104"/>
+      <c r="AB84" s="104"/>
+      <c r="AC84" s="104"/>
+      <c r="AD84" s="104"/>
+      <c r="AE84" s="104"/>
+      <c r="AF84" s="104"/>
+      <c r="AG84" s="104"/>
+      <c r="AH84" s="104"/>
+      <c r="AI84" s="104"/>
+      <c r="AJ84" s="104"/>
+      <c r="AK84" s="104"/>
+      <c r="AL84" s="104"/>
+      <c r="AM84" s="104"/>
+      <c r="AN84" s="104"/>
+      <c r="AO84" s="104"/>
+      <c r="AP84" s="104"/>
+      <c r="AQ84" s="104"/>
+      <c r="AR84" s="104"/>
+      <c r="AS84" s="104"/>
+      <c r="AT84" s="104"/>
+      <c r="AU84" s="104"/>
+      <c r="AV84" s="104"/>
+      <c r="AW84" s="104"/>
+      <c r="AX84" s="104"/>
+      <c r="AY84" s="104"/>
+      <c r="AZ84" s="104"/>
+      <c r="BA84" s="104"/>
+      <c r="BB84" s="104"/>
+      <c r="BC84" s="104"/>
+      <c r="BD84" s="104"/>
+      <c r="BE84" s="104"/>
+      <c r="BF84" s="104"/>
+      <c r="BG84" s="104"/>
+      <c r="BH84" s="104"/>
+      <c r="BI84" s="104"/>
+      <c r="BJ84" s="104"/>
+      <c r="BK84" s="104"/>
+      <c r="BL84" s="104"/>
+      <c r="BM84" s="104"/>
+      <c r="BN84" s="104"/>
+      <c r="BO84" s="104"/>
+      <c r="BP84" s="105"/>
       <c r="BQ84" s="38"/>
     </row>
     <row r="85" spans="1:69" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A85" s="87"/>
-      <c r="B85" s="87"/>
-      <c r="C85" s="87"/>
-      <c r="D85" s="87"/>
-      <c r="E85" s="87"/>
-      <c r="F85" s="87"/>
-      <c r="G85" s="87"/>
-      <c r="H85" s="87"/>
-      <c r="I85" s="87"/>
-      <c r="J85" s="87"/>
-      <c r="K85" s="87"/>
-      <c r="L85" s="87"/>
-      <c r="M85" s="87"/>
-      <c r="N85" s="87"/>
-      <c r="O85" s="87"/>
-      <c r="P85" s="87"/>
-      <c r="Q85" s="87"/>
-      <c r="R85" s="87"/>
-      <c r="S85" s="87"/>
-      <c r="T85" s="87"/>
-      <c r="U85" s="87"/>
-      <c r="V85" s="87"/>
-      <c r="W85" s="87"/>
-      <c r="X85" s="87"/>
-      <c r="Y85" s="87"/>
-      <c r="Z85" s="87"/>
-      <c r="AA85" s="87"/>
-      <c r="AB85" s="87"/>
-      <c r="AC85" s="87"/>
-      <c r="AD85" s="87"/>
-      <c r="AE85" s="87"/>
-      <c r="AF85" s="87"/>
-      <c r="AG85" s="87"/>
-      <c r="AH85" s="87"/>
-      <c r="AI85" s="87"/>
-      <c r="AJ85" s="87"/>
-      <c r="AK85" s="87"/>
-      <c r="AL85" s="87"/>
-      <c r="AM85" s="87"/>
-      <c r="AN85" s="87"/>
-      <c r="AO85" s="87"/>
-      <c r="AP85" s="87"/>
-      <c r="AQ85" s="87"/>
-      <c r="AR85" s="87"/>
-      <c r="AS85" s="87"/>
-      <c r="AT85" s="87"/>
-      <c r="AU85" s="87"/>
-      <c r="AV85" s="87"/>
-      <c r="AW85" s="87"/>
-      <c r="AX85" s="87"/>
-      <c r="AY85" s="87"/>
-      <c r="AZ85" s="87"/>
-      <c r="BA85" s="87"/>
-      <c r="BB85" s="87"/>
-      <c r="BC85" s="87"/>
-      <c r="BD85" s="87"/>
-      <c r="BE85" s="87"/>
-      <c r="BF85" s="87"/>
-      <c r="BG85" s="87"/>
-      <c r="BH85" s="87"/>
-      <c r="BI85" s="87"/>
-      <c r="BJ85" s="87"/>
-      <c r="BK85" s="87"/>
-      <c r="BL85" s="87"/>
-      <c r="BM85" s="87"/>
-      <c r="BN85" s="87"/>
-      <c r="BO85" s="87"/>
-      <c r="BP85" s="88"/>
+      <c r="A85" s="104"/>
+      <c r="B85" s="104"/>
+      <c r="C85" s="104"/>
+      <c r="D85" s="104"/>
+      <c r="E85" s="104"/>
+      <c r="F85" s="104"/>
+      <c r="G85" s="104"/>
+      <c r="H85" s="104"/>
+      <c r="I85" s="104"/>
+      <c r="J85" s="104"/>
+      <c r="K85" s="104"/>
+      <c r="L85" s="104"/>
+      <c r="M85" s="104"/>
+      <c r="N85" s="104"/>
+      <c r="O85" s="104"/>
+      <c r="P85" s="104"/>
+      <c r="Q85" s="104"/>
+      <c r="R85" s="104"/>
+      <c r="S85" s="104"/>
+      <c r="T85" s="104"/>
+      <c r="U85" s="104"/>
+      <c r="V85" s="104"/>
+      <c r="W85" s="104"/>
+      <c r="X85" s="104"/>
+      <c r="Y85" s="104"/>
+      <c r="Z85" s="104"/>
+      <c r="AA85" s="104"/>
+      <c r="AB85" s="104"/>
+      <c r="AC85" s="104"/>
+      <c r="AD85" s="104"/>
+      <c r="AE85" s="104"/>
+      <c r="AF85" s="104"/>
+      <c r="AG85" s="104"/>
+      <c r="AH85" s="104"/>
+      <c r="AI85" s="104"/>
+      <c r="AJ85" s="104"/>
+      <c r="AK85" s="104"/>
+      <c r="AL85" s="104"/>
+      <c r="AM85" s="104"/>
+      <c r="AN85" s="104"/>
+      <c r="AO85" s="104"/>
+      <c r="AP85" s="104"/>
+      <c r="AQ85" s="104"/>
+      <c r="AR85" s="104"/>
+      <c r="AS85" s="104"/>
+      <c r="AT85" s="104"/>
+      <c r="AU85" s="104"/>
+      <c r="AV85" s="104"/>
+      <c r="AW85" s="104"/>
+      <c r="AX85" s="104"/>
+      <c r="AY85" s="104"/>
+      <c r="AZ85" s="104"/>
+      <c r="BA85" s="104"/>
+      <c r="BB85" s="104"/>
+      <c r="BC85" s="104"/>
+      <c r="BD85" s="104"/>
+      <c r="BE85" s="104"/>
+      <c r="BF85" s="104"/>
+      <c r="BG85" s="104"/>
+      <c r="BH85" s="104"/>
+      <c r="BI85" s="104"/>
+      <c r="BJ85" s="104"/>
+      <c r="BK85" s="104"/>
+      <c r="BL85" s="104"/>
+      <c r="BM85" s="104"/>
+      <c r="BN85" s="104"/>
+      <c r="BO85" s="104"/>
+      <c r="BP85" s="105"/>
       <c r="BQ85" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AG2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:W9"/>
-    <mergeCell ref="BG10:BK10"/>
-    <mergeCell ref="BL10:BP10"/>
-    <mergeCell ref="AC10:AG10"/>
-    <mergeCell ref="AH10:AL10"/>
-    <mergeCell ref="AM10:AQ10"/>
-    <mergeCell ref="AR10:AV10"/>
-    <mergeCell ref="AW10:BA10"/>
     <mergeCell ref="A70:BP85"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
@@ -8820,6 +8791,25 @@
     <mergeCell ref="I10:M10"/>
     <mergeCell ref="N10:R10"/>
     <mergeCell ref="BB10:BF10"/>
+    <mergeCell ref="BG10:BK10"/>
+    <mergeCell ref="BL10:BP10"/>
+    <mergeCell ref="AC10:AG10"/>
+    <mergeCell ref="AH10:AL10"/>
+    <mergeCell ref="AM10:AQ10"/>
+    <mergeCell ref="AR10:AV10"/>
+    <mergeCell ref="AW10:BA10"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:W9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AG2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <conditionalFormatting sqref="H15:H69 H13">

</xml_diff>